<commit_message>
re-organize values of constant c
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8400" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="20145" windowHeight="7395" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data11" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,14 @@
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -550,155 +557,157 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1016,8 +1025,8 @@
   <sheetPr/>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="7"/>
@@ -1030,370 +1039,378 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="1">
+      <c r="A2" s="4">
         <v>7.734603659</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>-9.29974075</v>
       </c>
-      <c r="C2" s="1">
-        <f>B2+D2</f>
-        <v>-9.27945183302835</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.0202889169716493</v>
+      <c r="C2" s="4">
+        <f t="shared" ref="C2:C25" si="0">B2+D2</f>
+        <v>-9.27877112419782</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.0209696258021805</v>
       </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
         <v>7.398316544</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>-9.303271</v>
       </c>
-      <c r="C3" s="1">
-        <f>B3+D3</f>
-        <v>-9.2828467498425</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.0204242501574988</v>
+      <c r="C3" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.28217704928256</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.0210939507174438</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1">
+      <c r="A4" s="4">
         <v>7.06202942799999</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>-9.305298</v>
       </c>
-      <c r="C4" s="1">
-        <f>B4+D4</f>
-        <v>-9.28467633679579</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.0206216632042114</v>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.28401399136472</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.0212840086352783</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1">
+      <c r="A5" s="4">
         <v>6.99477200493787</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>-9.30541825</v>
       </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.28414069068237</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.0212775593176295</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1">
+      <c r="A6" s="4">
         <v>6.92751458181347</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>-9.305416</v>
       </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.305416</v>
+      </c>
+      <c r="D6" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1">
+      <c r="A7" s="4">
         <v>6.86025715868907</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>-9.305258</v>
       </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.28394005617462</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.0213179438253818</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>6.79299973556466</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>-9.30494375</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.28360454025992</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.0213392097400774</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1">
+      <c r="A9" s="4">
         <v>6.72574231244026</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>-9.30443575</v>
       </c>
-      <c r="C9" s="1">
-        <f>B9+D9</f>
-        <v>-9.28373072258981</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.0207050274101862</v>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.28085089283634</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.0235848571636644</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1">
+      <c r="A10" s="4">
         <v>6.65848488931586</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>-9.303711</v>
       </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.303711</v>
+      </c>
+      <c r="D10" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="1">
+      <c r="A11" s="4">
         <v>6.59122746619145</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>-9.3027445</v>
       </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.3027445</v>
+      </c>
+      <c r="D11" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="1">
+      <c r="A12" s="4">
         <v>6.52397004306705</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>-9.30149675</v>
       </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.30149675</v>
+      </c>
+      <c r="D12" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="1">
+      <c r="A13" s="4">
         <v>6.45671261994265</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>-9.29993175</v>
       </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.29993175</v>
+      </c>
+      <c r="D13" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="1">
+      <c r="A14" s="4">
         <v>6.389455197</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>-9.2980065</v>
       </c>
-      <c r="C14" s="1">
-        <f t="shared" ref="C14:C25" si="0">B14+D14</f>
-        <v>-9.27720872289682</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0.0207977771031755</v>
+      <c r="C14" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.2765447062902</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.0214617937098034</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="1">
+      <c r="A15" s="4">
         <v>6.05316808099999</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>-9.281312</v>
       </c>
-      <c r="C15" s="1">
-        <f t="shared" si="0"/>
-        <v>-9.26044924256136</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.0208627574386438</v>
+      <c r="C15" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.25981534941733</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.0214966505826721</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="1">
+      <c r="A16" s="4">
         <v>5.71688096599999</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>-9.24699775</v>
       </c>
-      <c r="C16" s="1">
-        <f t="shared" si="0"/>
-        <v>-9.22606542156227</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0.0209323284377305</v>
+      <c r="C16" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.22545581578752</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.0215419342124851</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="1">
+      <c r="A17" s="4">
         <v>5.38059385</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="3">
         <v>-9.18425575</v>
       </c>
-      <c r="C17" s="1">
-        <f t="shared" si="0"/>
-        <v>-9.16318770558089</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0.021068044419114</v>
+      <c r="C17" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.16266257845306</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.0215931715469442</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="1">
+      <c r="A18" s="4">
         <v>5.044306734</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="3">
         <v>-9.07655725</v>
       </c>
-      <c r="C18" s="1">
-        <f t="shared" si="0"/>
-        <v>-9.05542446500278</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0.0211327849972171</v>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.05490492455843</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.0216523254415718</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="1">
+      <c r="A19" s="4">
         <v>4.70801961899999</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="3">
         <v>-8.89676175</v>
       </c>
-      <c r="C19" s="1">
-        <f t="shared" si="0"/>
-        <v>-8.87558418799888</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0.0211775620011249</v>
+      <c r="C19" s="4">
+        <f t="shared" si="0"/>
+        <v>-8.87509644543177</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.0216653045682302</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="1">
+      <c r="A20" s="4">
         <v>4.37173250299999</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="3">
         <v>-8.610972</v>
       </c>
-      <c r="C20" s="1">
-        <f t="shared" si="0"/>
-        <v>-8.5902008496981</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0.0207711503018963</v>
+      <c r="C20" s="4">
+        <f t="shared" si="0"/>
+        <v>-8.58969112874629</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.021280871253706</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="1">
+      <c r="A21" s="4">
         <v>4.035445387</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="3">
         <v>-8.184804</v>
       </c>
-      <c r="C21" s="1">
-        <f t="shared" si="0"/>
-        <v>-8.16517022436926</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0.019633775630742</v>
+      <c r="C21" s="4">
+        <f t="shared" si="0"/>
+        <v>-8.1644223392305</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.0203816607694967</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="1">
+      <c r="A22" s="4">
         <v>3.69915827100001</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="3">
         <v>-7.561232</v>
       </c>
-      <c r="C22" s="1">
-        <f t="shared" si="0"/>
-        <v>-7.54303748961431</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0.0181945103856859</v>
+      <c r="C22" s="4">
+        <f t="shared" si="0"/>
+        <v>-7.54245840350752</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.0187735964924786</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="1">
+      <c r="A23" s="4">
         <v>3.36287115500002</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="3">
         <v>-6.6218255</v>
       </c>
-      <c r="C23" s="1">
-        <f t="shared" si="0"/>
-        <v>-6.60305319784747</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0.0187723021525279</v>
+      <c r="C23" s="4">
+        <f t="shared" si="0"/>
+        <v>-6.60562327498075</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.0162022250192528</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="1">
+      <c r="A24" s="4">
         <v>3.02658403900003</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="3">
         <v>-5.380071</v>
       </c>
-      <c r="C24" s="1">
-        <f t="shared" si="0"/>
-        <v>-5.36170195460927</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0.0183690453907337</v>
+      <c r="C24" s="4">
+        <f t="shared" si="0"/>
+        <v>-5.36397948973004</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.0160915102699602</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="1">
+      <c r="A25" s="4">
         <v>2.69029692300004</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="3">
         <v>-3.654861</v>
       </c>
-      <c r="C25" s="1">
-        <f t="shared" si="0"/>
-        <v>-3.63993343623513</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0.0149275637648665</v>
+      <c r="C25" s="4">
+        <f t="shared" si="0"/>
+        <v>-3.63930487592718</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.0155561240728216</v>
       </c>
     </row>
   </sheetData>
@@ -1408,7 +1425,7 @@
   <sheetPr/>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
3 plot for the Aug 31st ppt
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -173,10 +173,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -194,9 +194,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -209,27 +215,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -238,9 +223,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,60 +240,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -332,7 +263,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -344,6 +307,43 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -360,13 +360,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -378,24 +480,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -408,25 +492,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,31 +510,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,67 +534,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,6 +557,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -572,17 +587,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -620,188 +640,165 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1128,7 +1125,7 @@
     <col min="1" max="1" width="19.25" customWidth="1"/>
     <col min="2" max="2" width="12.625"/>
     <col min="3" max="3" width="13.75"/>
-    <col min="4" max="4" width="12.625" style="2"/>
+    <col min="4" max="4" width="12.625"/>
     <col min="5" max="5" width="12.625"/>
     <col min="8" max="10" width="12.625"/>
   </cols>
@@ -1151,111 +1148,111 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="7">
+      <c r="A2" s="2">
         <v>7.734603659</v>
       </c>
       <c r="B2">
         <v>-9.29974075</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="2">
         <f t="shared" ref="C2:C25" si="0">B2+E2</f>
         <v>-9.27877112419782</v>
       </c>
-      <c r="D2" s="4">
-        <v>0</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
         <v>0.0209696258021805</v>
       </c>
-      <c r="I2" s="7"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="7">
+      <c r="A3" s="2">
         <v>7.398316544</v>
       </c>
       <c r="B3">
         <v>-9.303271</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="2">
         <f t="shared" si="0"/>
         <v>-9.28217704928256</v>
       </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7">
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
         <v>0.0210939507174438</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="7">
+      <c r="A4" s="2">
         <v>7.06202942799999</v>
       </c>
       <c r="B4">
         <v>-9.305298</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="2">
         <f t="shared" si="0"/>
         <v>-9.28401399136472</v>
       </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7">
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
         <v>0.0212840086352783</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="7">
+      <c r="A5" s="2">
         <v>6.99477200493787</v>
       </c>
       <c r="B5">
         <v>-9.30541825</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>-9.28414069068237</v>
       </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="7">
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
         <v>0.0212775593176295</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="7">
+      <c r="A6" s="2">
         <v>6.92751458181347</v>
       </c>
       <c r="B6">
         <v>-9.305416</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="2">
         <f t="shared" si="0"/>
         <v>-9.305416</v>
       </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="7">
+      <c r="A7" s="2">
         <v>6.86025715868907</v>
       </c>
       <c r="B7">
         <v>-9.305258</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="2">
         <f t="shared" si="0"/>
         <v>-9.28394005617462</v>
       </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7">
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
         <v>0.0213179438253818</v>
       </c>
     </row>
@@ -1266,11 +1263,11 @@
       <c r="B8">
         <v>-9.30494375</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>-9.28360454025992</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>0</v>
       </c>
       <c r="E8">
@@ -1278,308 +1275,308 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="7">
+      <c r="A9" s="2">
         <v>6.72574231244026</v>
       </c>
       <c r="B9">
         <v>-9.30443575</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>-9.28085089283634</v>
       </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="7">
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
         <v>0.0235848571636644</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="7">
+      <c r="A10" s="2">
         <v>6.65848488931586</v>
       </c>
       <c r="B10">
         <v>-9.303711</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>-9.303711</v>
       </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="7">
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="7">
+      <c r="A11" s="2">
         <v>6.59122746619145</v>
       </c>
       <c r="B11">
         <v>-9.3027445</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>-9.3027445</v>
       </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="7">
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="7">
+      <c r="A12" s="2">
         <v>6.52397004306705</v>
       </c>
       <c r="B12">
         <v>-9.30149675</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>-9.30149675</v>
       </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7">
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="7">
+      <c r="A13" s="2">
         <v>6.45671261994265</v>
       </c>
       <c r="B13">
         <v>-9.29993175</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>-9.29993175</v>
       </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13" s="7">
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="7">
+      <c r="A14" s="2">
         <v>6.389455197</v>
       </c>
       <c r="B14">
         <v>-9.2980065</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>-9.2765447062902</v>
       </c>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7">
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
         <v>0.0214617937098034</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="7">
+      <c r="A15" s="2">
         <v>6.05316808099999</v>
       </c>
       <c r="B15">
         <v>-9.281312</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>-9.25981534941733</v>
       </c>
-      <c r="D15" s="4">
-        <v>0</v>
-      </c>
-      <c r="E15" s="7">
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
         <v>0.0214966505826721</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="7">
+      <c r="A16" s="2">
         <v>5.71688096599999</v>
       </c>
       <c r="B16">
         <v>-9.24699775</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>-9.22545581578752</v>
       </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" s="7">
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
         <v>0.0215419342124851</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="7">
+      <c r="A17" s="2">
         <v>5.38059385</v>
       </c>
       <c r="B17">
         <v>-9.18425575</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>-9.16266257845306</v>
       </c>
-      <c r="D17" s="4">
-        <v>0</v>
-      </c>
-      <c r="E17" s="7">
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
         <v>0.0215931715469442</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="7">
+      <c r="A18" s="2">
         <v>5.044306734</v>
       </c>
       <c r="B18">
         <v>-9.07655725</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>-9.05490492455843</v>
       </c>
-      <c r="D18" s="4">
-        <v>0</v>
-      </c>
-      <c r="E18" s="7">
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
         <v>0.0216523254415718</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="7">
+      <c r="A19" s="2">
         <v>4.70801961899999</v>
       </c>
       <c r="B19">
         <v>-8.89676175</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>-8.87509644543177</v>
       </c>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="7">
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
         <v>0.0216653045682302</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="7">
+      <c r="A20" s="2">
         <v>4.37173250299999</v>
       </c>
       <c r="B20">
         <v>-8.610972</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>-8.58969112874629</v>
       </c>
-      <c r="D20" s="4">
-        <v>0</v>
-      </c>
-      <c r="E20" s="7">
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2">
         <v>0.021280871253706</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="7">
+      <c r="A21" s="2">
         <v>4.035445387</v>
       </c>
       <c r="B21">
         <v>-8.184804</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>-8.1644223392305</v>
       </c>
-      <c r="D21" s="4">
-        <v>0</v>
-      </c>
-      <c r="E21" s="7">
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2">
         <v>0.0203816607694967</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="7">
+      <c r="A22" s="2">
         <v>3.69915827100001</v>
       </c>
       <c r="B22">
         <v>-7.561232</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>-7.54245840350752</v>
       </c>
-      <c r="D22" s="4">
-        <v>0</v>
-      </c>
-      <c r="E22" s="7">
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2">
         <v>0.0187735964924786</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="7">
+      <c r="A23" s="2">
         <v>3.36287115500002</v>
       </c>
       <c r="B23">
         <v>-6.6218255</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>-6.60562327498075</v>
       </c>
-      <c r="D23" s="4">
-        <v>0</v>
-      </c>
-      <c r="E23" s="7">
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2">
         <v>0.0162022250192528</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="7">
+      <c r="A24" s="2">
         <v>3.02658403900003</v>
       </c>
       <c r="B24">
         <v>-5.380071</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>-5.36397948973004</v>
       </c>
-      <c r="D24" s="4">
-        <v>0</v>
-      </c>
-      <c r="E24" s="7">
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
         <v>0.0160915102699602</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="7">
+      <c r="A25" s="2">
         <v>2.69029692300004</v>
       </c>
       <c r="B25">
         <v>-3.654861</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>-3.63930487592718</v>
       </c>
-      <c r="D25" s="4">
-        <v>0</v>
-      </c>
-      <c r="E25" s="7">
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2">
         <v>0.0155561240728216</v>
       </c>
     </row>
@@ -1590,28 +1587,28 @@
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="4:4">
-      <c r="D30" s="4"/>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" spans="4:4">
-      <c r="D31" s="4"/>
+      <c r="D31" s="3"/>
     </row>
     <row r="32" spans="4:4">
-      <c r="D32" s="4"/>
+      <c r="D32" s="3"/>
     </row>
     <row r="33" spans="4:4">
-      <c r="D33" s="4"/>
+      <c r="D33" s="3"/>
     </row>
     <row r="34" spans="4:4">
-      <c r="D34" s="4"/>
+      <c r="D34" s="3"/>
     </row>
     <row r="35" spans="4:4">
-      <c r="D35" s="4"/>
+      <c r="D35" s="3"/>
     </row>
     <row r="36" spans="4:4">
-      <c r="D36" s="4"/>
+      <c r="D36" s="3"/>
     </row>
     <row r="37" spans="4:4">
-      <c r="D37" s="4"/>
+      <c r="D37" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1626,7 +1623,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:G13"/>
+      <selection activeCell="F4" sqref="F4:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="6"/>
@@ -1660,44 +1657,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="1" spans="1:7">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3">
+    <row r="2" customFormat="1" spans="2:7">
+      <c r="B2" s="2">
         <v>7.62651333736756</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>-9.35571075</v>
       </c>
-      <c r="D2" s="4">
-        <f t="shared" ref="D2:D27" si="0">C2+F2</f>
+      <c r="D2" s="3">
+        <f t="shared" ref="D2:D29" si="0">C2+F2</f>
         <v>-9.35571075</v>
       </c>
-      <c r="E2" s="4">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="1" spans="1:7">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3">
+    <row r="3" customFormat="1" spans="2:7">
+      <c r="B3" s="2">
         <v>7.29492580096027</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>-9.36041425</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <f t="shared" si="0"/>
         <v>-9.36041425</v>
       </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
         <v>0</v>
       </c>
       <c r="G3">
@@ -1705,551 +1700,551 @@
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:7">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>7.0959732791159</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>-9.36272175</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <f t="shared" si="0"/>
         <v>-9.34142444866186</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>-1.74798</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <v>0.0212973013381394</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>0.0206405764390277</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:7">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>7.02965577183444</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>-9.36334625</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <f t="shared" si="0"/>
         <v>-9.34203116612822</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>-1.37949</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="4">
         <v>0.0213150838717795</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <v>0.02066163725461</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:7">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>6.96333826455299</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>-9.36387875</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <f t="shared" si="0"/>
         <v>-9.34252731341168</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>-0.649711</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="4">
         <v>0.0213514365883235</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="4">
         <v>0.0206943201157467</v>
       </c>
     </row>
     <row r="7" customFormat="1" spans="1:7">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>6.89702075727153</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>-9.364291</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <f t="shared" si="0"/>
         <v>-9.34292050564871</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>-0.436941</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="4">
         <v>0.0213704943512894</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="4">
         <v>0.0207214062522322</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:7">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>6.83070324999007</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>-9.36458075</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>-9.34319526886993</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>-0.194466</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="4">
         <v>0.0213854811300705</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="4">
         <v>0.0207224978899954</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="1:7">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>6.76438574270861</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>-9.36471925</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
         <v>-9.34329465155856</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>0.083872</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="4">
         <v>0.0214245984414376</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="4">
         <v>0.0207691221463404</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="1:7">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10">
         <v>6.69806823542716</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>-9.364684</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>-9.34324236527863</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>0.40474</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="4">
         <v>0.0214416347213709</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="4">
         <v>0.0207971474890624</v>
       </c>
     </row>
     <row r="11" customFormat="1" spans="1:7">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>6.6317507281457</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>-9.36446125</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <f t="shared" si="0"/>
         <v>-9.34298510923149</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>0.766066</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="4">
         <v>0.0214761407685137</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="4">
         <v>0.0208237304654679</v>
       </c>
     </row>
     <row r="12" customFormat="1" spans="1:7">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>6.56543322086424</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <v>-9.36401425</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <f t="shared" si="0"/>
         <v>-9.3425189263749</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>1.209655</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="4">
         <v>0.0214953236250955</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="4">
         <v>0.0208437353704383</v>
       </c>
     </row>
     <row r="13" customFormat="1" spans="1:7">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>6.49911571358279</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>-9.363318</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <f t="shared" si="0"/>
         <v>-9.34181344827522</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>1.650845</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="4">
         <v>0.0215045517247771</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="4">
         <v>0.0208632790939217</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="1:7">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>6.43279820630133</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <v>-9.36232725</v>
       </c>
-      <c r="D14" s="4">
-        <f t="shared" si="0"/>
-        <v>-9.36232725</v>
-      </c>
-      <c r="E14" s="4">
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>-9.34080128378352</v>
+      </c>
+      <c r="E14" s="3">
         <v>2.184954</v>
       </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
+      <c r="F14" s="4">
+        <v>0.0215259662164836</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.0208786517777622</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="1:7">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>6.36648069901987</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
         <v>-9.3610255</v>
       </c>
-      <c r="D15" s="4">
-        <f t="shared" si="0"/>
-        <v>-9.3610255</v>
-      </c>
-      <c r="E15" s="4">
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>-9.33948007495655</v>
+      </c>
+      <c r="E15" s="3">
         <v>2.81936</v>
       </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
+      <c r="F15" s="4">
+        <v>0.0215454250434452</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0.0209155631075892</v>
       </c>
     </row>
     <row r="16" customFormat="1" spans="1:7">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>6.30016319173841</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
         <v>-9.359363</v>
       </c>
-      <c r="D16" s="4">
-        <f t="shared" si="0"/>
-        <v>-9.359363</v>
-      </c>
-      <c r="E16" s="4">
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>-9.33780344436616</v>
+      </c>
+      <c r="E16" s="3">
         <v>3.470399</v>
       </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
+      <c r="F16" s="4">
+        <v>0.02155955563384</v>
+      </c>
+      <c r="G16" s="4">
+        <v>0.02093910836919</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:7">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17">
         <v>6.23384568445696</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <v>-9.3572985</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <f t="shared" si="0"/>
         <v>-9.33572266567675</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>8.313759</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="4">
         <v>0.0215758343232551</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="4">
         <v>0.0209624503779583</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="1:7">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18">
         <v>6.1675281771755</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18">
         <v>-9.35477725</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <f t="shared" si="0"/>
         <v>-9.33318746929334</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>16.364584</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="4">
         <v>0.0215897807066604</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="4">
         <v>0.0209664669130575</v>
       </c>
     </row>
     <row r="19" customFormat="1" spans="1:6">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>5.96857565533113</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19">
         <v>-9.3439195</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <f t="shared" si="0"/>
         <v>-9.3439195</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>29.162834</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19">
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="1:6">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>5.63698811892385</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20">
         <v>-9.31057675</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <f t="shared" si="0"/>
         <v>-9.31057675</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>49.590418</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="1" spans="1:6">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>5.30540058251656</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21">
         <v>-9.2470915</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <f t="shared" si="0"/>
         <v>-9.2470915</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>81.795232</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21">
         <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="1" spans="1:6">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>4.97381304610928</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22">
         <v>-9.13348925</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <f t="shared" si="0"/>
         <v>-9.13348925</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>126.264436</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="1" spans="1:6">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>4.64222550970199</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23">
         <v>-8.9380785</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <f t="shared" si="0"/>
         <v>-8.9380785</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <v>184.537527</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23">
         <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="1" spans="1:6">
-      <c r="A24" s="2" t="s">
+      <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>4.31063797329471</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24">
         <v>-8.63161825</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <f t="shared" si="0"/>
         <v>-8.63161825</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="3">
         <v>278.177108</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24">
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="1" spans="1:6">
-      <c r="A25" s="2" t="s">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>3.97905043688742</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25">
         <v>-8.18573275</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <f t="shared" si="0"/>
         <v>-8.18573275</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="3">
         <v>410.94174</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="2" t="s">
+      <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>3.64746290048014</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26">
         <v>-7.534209</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="3">
         <f t="shared" si="0"/>
         <v>-7.534209</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26">
         <v>515.291824</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>3.31587536407285</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27">
         <v>-6.56529875</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="3">
         <f t="shared" si="0"/>
         <v>-6.56529875</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27">
         <v>765.428943</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27">
         <v>0</v>
       </c>
     </row>
@@ -2257,20 +2252,20 @@
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="3">
         <v>2.98428782766557</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28">
         <v>-5.3080285</v>
       </c>
-      <c r="D28" s="6">
-        <f>C28+F28</f>
+      <c r="D28" s="3">
+        <f t="shared" si="0"/>
         <v>-5.3080285</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="3">
         <v>0</v>
       </c>
     </row>
@@ -2278,46 +2273,46 @@
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="3">
         <v>2.65270029125828</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29">
         <v>-3.53590775</v>
       </c>
-      <c r="D29" s="6">
-        <f>C29+F29</f>
+      <c r="D29" s="3">
+        <f t="shared" si="0"/>
         <v>-3.53590775</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="5:5">
-      <c r="E30" s="4"/>
+      <c r="E30" s="3"/>
     </row>
     <row r="31" spans="5:5">
-      <c r="E31" s="4"/>
+      <c r="E31" s="3"/>
     </row>
     <row r="32" spans="5:5">
-      <c r="E32" s="4"/>
+      <c r="E32" s="3"/>
     </row>
     <row r="33" spans="5:5">
-      <c r="E33" s="4"/>
+      <c r="E33" s="3"/>
     </row>
     <row r="34" spans="5:5">
-      <c r="E34" s="4"/>
+      <c r="E34" s="3"/>
     </row>
     <row r="35" spans="5:5">
-      <c r="E35" s="4"/>
+      <c r="E35" s="3"/>
     </row>
     <row r="36" spans="5:5">
-      <c r="E36" s="4"/>
+      <c r="E36" s="3"/>
     </row>
     <row r="37" spans="5:5">
-      <c r="E37" s="4"/>
+      <c r="E37" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
plot for optimized LJ and X6
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="740" windowWidth="24880" windowHeight="15540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="6060" yWindow="3540" windowWidth="24680" windowHeight="15540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data11" sheetId="1" r:id="rId1"/>
@@ -1750,7 +1750,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="G2" sqref="G2:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1807,13 +1807,13 @@
         <v>-0.48899999999999999</v>
       </c>
       <c r="G2">
-        <v>0.22700000000000001</v>
+        <v>-1.1224000000000001</v>
       </c>
       <c r="H2">
         <v>-0.43709999999999999</v>
       </c>
       <c r="I2">
-        <v>0.22750000000000001</v>
+        <v>-1.1273</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1836,13 +1836,13 @@
         <v>-0.50070000000000003</v>
       </c>
       <c r="G3">
-        <v>0.22689999999999999</v>
+        <v>-1.1551</v>
       </c>
       <c r="H3">
         <v>-0.44840000000000002</v>
       </c>
       <c r="I3">
-        <v>0.22739999999999999</v>
+        <v>-1.1593</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1865,13 +1865,13 @@
         <v>-0.51090000000000002</v>
       </c>
       <c r="G4">
-        <v>0.2268</v>
+        <v>-1.1852</v>
       </c>
       <c r="H4">
         <v>-0.4582</v>
       </c>
       <c r="I4">
-        <v>0.2273</v>
+        <v>-1.1886000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1894,13 +1894,13 @@
         <v>-0.51939999999999997</v>
       </c>
       <c r="G5">
-        <v>0.22670000000000001</v>
+        <v>-1.2121999999999999</v>
       </c>
       <c r="H5">
         <v>-0.46600000000000003</v>
       </c>
       <c r="I5">
-        <v>0.2273</v>
+        <v>-1.2143999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1923,13 +1923,13 @@
         <v>-0.52569999999999995</v>
       </c>
       <c r="G6">
-        <v>0.2266</v>
+        <v>-1.2352000000000001</v>
       </c>
       <c r="H6">
         <v>-0.47139999999999999</v>
       </c>
       <c r="I6">
-        <v>0.22720000000000001</v>
+        <v>-1.2361</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1952,13 +1952,13 @@
         <v>-0.52949999999999997</v>
       </c>
       <c r="G7">
-        <v>0.22650000000000001</v>
+        <v>-1.2532000000000001</v>
       </c>
       <c r="H7">
         <v>-0.47389999999999999</v>
       </c>
       <c r="I7">
-        <v>0.2271</v>
+        <v>-1.2525999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1981,13 +1981,13 @@
         <v>-0.53010000000000002</v>
       </c>
       <c r="G8">
-        <v>0.22639999999999999</v>
+        <v>-1.2652000000000001</v>
       </c>
       <c r="H8">
         <v>-0.47289999999999999</v>
       </c>
       <c r="I8">
-        <v>0.2271</v>
+        <v>-1.2632000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -2010,13 +2010,13 @@
         <v>-0.52690000000000003</v>
       </c>
       <c r="G9">
-        <v>0.22620000000000001</v>
+        <v>-1.27</v>
       </c>
       <c r="H9">
         <v>-0.46760000000000002</v>
       </c>
       <c r="I9">
-        <v>0.22700000000000001</v>
+        <v>-1.2665</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -2039,13 +2039,13 @@
         <v>-0.51939999999999997</v>
       </c>
       <c r="G10">
-        <v>0.2261</v>
+        <v>-1.266</v>
       </c>
       <c r="H10">
         <v>-0.4572</v>
       </c>
       <c r="I10">
-        <v>0.22689999999999999</v>
+        <v>-1.2613000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -2068,13 +2068,13 @@
         <v>-0.50649999999999995</v>
       </c>
       <c r="G11">
-        <v>0.22600000000000001</v>
+        <v>-1.2516</v>
       </c>
       <c r="H11">
         <v>-0.44080000000000003</v>
       </c>
       <c r="I11">
-        <v>0.2268</v>
+        <v>-1.2462</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -2097,13 +2097,13 @@
         <v>-0.4874</v>
       </c>
       <c r="G12">
-        <v>0.2258</v>
+        <v>-1.2246999999999999</v>
       </c>
       <c r="H12">
         <v>-0.4173</v>
       </c>
       <c r="I12">
-        <v>0.22670000000000001</v>
+        <v>-1.2194</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -2126,13 +2126,13 @@
         <v>-0.46100000000000002</v>
       </c>
       <c r="G13">
-        <v>0.22570000000000001</v>
+        <v>-1.1832</v>
       </c>
       <c r="H13">
         <v>-0.38540000000000002</v>
       </c>
       <c r="I13">
-        <v>0.2266</v>
+        <v>-1.1791</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -2155,13 +2155,13 @@
         <v>-0.4259</v>
       </c>
       <c r="G14">
-        <v>0.22550000000000001</v>
+        <v>-1.1243000000000001</v>
       </c>
       <c r="H14">
         <v>-0.34350000000000003</v>
       </c>
       <c r="I14">
-        <v>0.22650000000000001</v>
+        <v>-1.1232</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2184,13 +2184,13 @@
         <v>-0.38069999999999998</v>
       </c>
       <c r="G15">
-        <v>0.22539999999999999</v>
+        <v>-1.0448999999999999</v>
       </c>
       <c r="H15">
         <v>-0.29020000000000001</v>
       </c>
       <c r="I15">
-        <v>0.2263</v>
+        <v>-1.0491999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -2213,13 +2213,13 @@
         <v>-0.3236</v>
       </c>
       <c r="G16">
-        <v>0.22520000000000001</v>
+        <v>-0.94140000000000001</v>
       </c>
       <c r="H16">
         <v>-0.2233</v>
       </c>
       <c r="I16">
-        <v>0.22620000000000001</v>
+        <v>-0.95450000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data for VopX and VopFull
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370" tabRatio="500" activeTab="2"/>
+    <workbookView windowWidth="20385" windowHeight="7950" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data11" sheetId="1" r:id="rId1"/>
@@ -236,8 +236,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -250,17 +250,18 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -273,7 +274,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -281,37 +289,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -325,39 +303,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -378,9 +325,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -393,8 +348,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -415,7 +415,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,7 +523,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,19 +547,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,91 +571,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -565,31 +589,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -607,16 +607,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -636,17 +627,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -666,15 +662,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -690,161 +677,174 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -912,8 +912,8 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
     </queryTableFields>
@@ -932,8 +932,8 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
     </queryTableFields>
@@ -2402,8 +2402,8 @@
   <sheetPr/>
   <dimension ref="A1:L16384"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -2480,13 +2480,13 @@
         <v>-1.1506</v>
       </c>
       <c r="J2" s="1">
-        <v>-1.1688</v>
+        <v>-1.1655</v>
       </c>
       <c r="K2">
         <v>-1.1812</v>
       </c>
       <c r="L2">
-        <v>-1.053</v>
+        <v>-1.1634</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:12">
@@ -2518,13 +2518,13 @@
         <v>-1.175</v>
       </c>
       <c r="J3" s="1">
-        <v>-1.1889</v>
+        <v>-1.1862</v>
       </c>
       <c r="K3">
         <v>-1.2007</v>
       </c>
       <c r="L3">
-        <v>-1.0879</v>
+        <v>-1.1845</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:12">
@@ -2556,13 +2556,13 @@
         <v>-1.1968</v>
       </c>
       <c r="J4" s="1">
-        <v>-1.2066</v>
+        <v>-1.2046</v>
       </c>
       <c r="K4">
         <v>-1.2173</v>
       </c>
       <c r="L4">
-        <v>-1.1236</v>
+        <v>-1.2032</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:12">
@@ -2594,13 +2594,13 @@
         <v>-1.2154</v>
       </c>
       <c r="J5" s="1">
-        <v>-1.2213</v>
+        <v>-1.22</v>
       </c>
       <c r="K5">
         <v>-1.2304</v>
       </c>
       <c r="L5">
-        <v>-1.16</v>
+        <v>-1.219</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:12">
@@ -2632,13 +2632,13 @@
         <v>-1.2303</v>
       </c>
       <c r="J6" s="1">
-        <v>-1.2326</v>
+        <v>-1.232</v>
       </c>
       <c r="K6">
         <v>-1.2394</v>
       </c>
       <c r="L6">
-        <v>-1.197</v>
+        <v>-1.2314</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:12">
@@ -2670,13 +2670,13 @@
         <v>-1.2406</v>
       </c>
       <c r="J7" s="1">
-        <v>-1.2398</v>
+        <v>-1.2399</v>
       </c>
       <c r="K7">
         <v>-1.2435</v>
       </c>
       <c r="L7">
-        <v>-1.2345</v>
+        <v>-1.2398</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:12">
@@ -2708,13 +2708,13 @@
         <v>-1.2456</v>
       </c>
       <c r="J8" s="1">
-        <v>-1.2423</v>
+        <v>-1.243</v>
       </c>
       <c r="K8">
         <v>-1.2419</v>
       </c>
       <c r="L8">
-        <v>-1.2722</v>
+        <v>-1.2434</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:12">
@@ -2746,13 +2746,13 @@
         <v>-1.2443</v>
       </c>
       <c r="J9" s="1">
-        <v>-1.2394</v>
+        <v>-1.2405</v>
       </c>
       <c r="K9">
         <v>-1.2337</v>
       </c>
       <c r="L9">
-        <v>-1.3096</v>
+        <v>-1.2414</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:12">
@@ -2784,13 +2784,13 @@
         <v>-1.2357</v>
       </c>
       <c r="J10" s="1">
-        <v>-1.2301</v>
+        <v>-1.2314</v>
       </c>
       <c r="K10">
         <v>-1.2176</v>
       </c>
       <c r="L10">
-        <v>-1.3454</v>
+        <v>-1.2329</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:12">
@@ -2822,13 +2822,13 @@
         <v>-1.2185</v>
       </c>
       <c r="J11" s="1">
-        <v>-1.2134</v>
+        <v>-1.2149</v>
       </c>
       <c r="K11">
         <v>-1.1925</v>
       </c>
       <c r="L11">
-        <v>-1.3768</v>
+        <v>-1.2169</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:12">
@@ -2860,13 +2860,13 @@
         <v>-1.1915</v>
       </c>
       <c r="J12" s="1">
-        <v>-1.1884</v>
+        <v>-1.1895</v>
       </c>
       <c r="K12">
         <v>-1.1569</v>
       </c>
       <c r="L12">
-        <v>-1.3978</v>
+        <v>-1.1921</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:12">
@@ -2898,13 +2898,13 @@
         <v>-1.1531</v>
       </c>
       <c r="J13" s="1">
-        <v>-1.1536</v>
+        <v>-1.1541</v>
       </c>
       <c r="K13">
         <v>-1.1092</v>
       </c>
       <c r="L13">
-        <v>-1.396</v>
+        <v>-1.1572</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:12">
@@ -2936,13 +2936,13 @@
         <v>-1.1017</v>
       </c>
       <c r="J14" s="1">
-        <v>-1.1078</v>
+        <v>-1.107</v>
       </c>
       <c r="K14">
         <v>-1.0475</v>
       </c>
       <c r="L14">
-        <v>-1.346</v>
+        <v>-1.1107</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:12">
@@ -2974,13 +2974,13 @@
         <v>-1.0353</v>
       </c>
       <c r="J15" s="1">
-        <v>-1.0494</v>
+        <v>-1.0466</v>
       </c>
       <c r="K15">
         <v>-0.9697</v>
       </c>
       <c r="L15">
-        <v>-1.1961</v>
+        <v>-1.0507</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:12">
@@ -3012,13 +3012,13 @@
         <v>-0.9518</v>
       </c>
       <c r="J16" s="1">
-        <v>-0.9765</v>
+        <v>-0.9708</v>
       </c>
       <c r="K16">
         <v>-0.8734</v>
       </c>
       <c r="L16">
-        <v>-0.8435</v>
+        <v>-0.9754</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1"/>

</xml_diff>

<commit_message>
update data X6 potential
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -235,23 +235,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -273,31 +265,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,6 +289,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -319,7 +312,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -335,7 +328,58 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -349,52 +393,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -415,67 +415,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,13 +463,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,19 +523,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -535,25 +541,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -565,7 +553,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,19 +583,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -600,15 +600,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -638,11 +629,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -700,151 +689,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -912,8 +912,8 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
     </queryTableFields>
@@ -932,8 +932,8 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
     </queryTableFields>
@@ -2403,7 +2403,7 @@
   <dimension ref="A1:L16384"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
add phonons in QM calculation data
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -12,9 +12,9 @@
     <sheet name="CCmd" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="tmp" localSheetId="2">CCmd!$K$2:$K$16</definedName>
-    <definedName name="tmp_1" localSheetId="2">CCmd!$J$2:$J$16</definedName>
-    <definedName name="ExternalData_1" localSheetId="2">CCmd!$L$2:$L$16</definedName>
+    <definedName name="tmp" localSheetId="2">CCmd!$L$2:$L$16</definedName>
+    <definedName name="tmp_1" localSheetId="2">CCmd!$K$2:$K$16</definedName>
+    <definedName name="ExternalData_1" localSheetId="2">CCmd!$M$2:$M$16</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46">
   <si>
     <t>C(A)</t>
   </si>
@@ -203,6 +203,9 @@
     <t>QM</t>
   </si>
   <si>
+    <t>QM-phn</t>
+  </si>
+  <si>
     <t>X6S</t>
   </si>
   <si>
@@ -249,19 +252,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -274,13 +268,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -288,10 +275,40 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -305,7 +322,23 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -313,14 +346,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -335,37 +360,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -378,8 +381,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -392,9 +396,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -409,55 +412,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,13 +448,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,85 +460,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,7 +508,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -603,17 +606,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -627,25 +624,31 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -667,16 +670,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -703,148 +706,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -912,8 +915,8 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
     </queryTableFields>
@@ -932,8 +935,8 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
     </queryTableFields>
@@ -2400,22 +2403,23 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:L16384"/>
+  <dimension ref="A1:M16384"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="4" max="4" width="12.8333333333333" customWidth="1"/>
-    <col min="6" max="6" width="11.3333333333333" customWidth="1"/>
-    <col min="8" max="8" width="11.8333333333333" customWidth="1"/>
-    <col min="10" max="11" width="7.66666666666667" customWidth="1"/>
-    <col min="12" max="12" width="16.25" customWidth="1"/>
+    <col min="4" max="4" width="13.75"/>
+    <col min="5" max="5" width="12.8333333333333" customWidth="1"/>
+    <col min="7" max="7" width="11.3333333333333" customWidth="1"/>
+    <col min="9" max="9" width="11.8333333333333" customWidth="1"/>
+    <col min="11" max="12" width="7.66666666666667" customWidth="1"/>
+    <col min="13" max="13" width="16.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:12">
+    <row r="1" s="1" customFormat="1" spans="1:13">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>34</v>
@@ -2447,11 +2451,14 @@
       <c r="K1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:12">
+    <row r="2" s="1" customFormat="1" spans="1:13">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -2461,35 +2468,38 @@
       <c r="C2" s="1">
         <v>-1.19325000000003</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
+        <v>-1.13525366887779</v>
+      </c>
+      <c r="E2" s="3">
         <v>-0.4985</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>-1.1389</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>-0.5643</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>-1.1224</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>-0.5127</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>-1.1506</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>-1.1655</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>-1.1812</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>-1.1634</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:12">
+    <row r="3" s="1" customFormat="1" spans="1:13">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2499,35 +2509,38 @@
       <c r="C3" s="1">
         <v>-1.20764865951742</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
+        <v>-1.14924232896001</v>
+      </c>
+      <c r="E3" s="3">
         <v>-0.509</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>-1.1675</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>-0.5759</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>-1.1551</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>-0.524</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>-1.175</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>-1.1862</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>-1.2007</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>-1.1845</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" spans="1:12">
+    <row r="4" s="1" customFormat="1" spans="1:13">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -2537,35 +2550,38 @@
       <c r="C4" s="1">
         <v>-1.21992613941021</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
+        <v>-1.16068164970457</v>
+      </c>
+      <c r="E4" s="3">
         <v>-0.5176</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>-1.1937</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>-0.586</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>-1.1852</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>-0.5337</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>-1.1968</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>-1.2046</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>-1.2173</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>-1.2032</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" spans="1:12">
+    <row r="5" s="1" customFormat="1" spans="1:13">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -2575,35 +2591,38 @@
       <c r="C5" s="1">
         <v>-1.22943109919572</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
+        <v>-1.16974720798473</v>
+      </c>
+      <c r="E5" s="3">
         <v>-0.5239</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>-1.2169</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>-0.5944</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>-1.2122</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>-0.5414</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>-1.2154</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>-1.22</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>-1.2304</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>-1.219</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" spans="1:12">
+    <row r="6" s="1" customFormat="1" spans="1:13">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -2613,35 +2632,38 @@
       <c r="C6" s="1">
         <v>-1.2361116621984</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
+        <v>-1.1760822313158</v>
+      </c>
+      <c r="E6" s="3">
         <v>-0.5273</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>-1.2365</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>-0.6007</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>-1.2352</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>-0.5467</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>-1.2303</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>-1.232</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>-1.2394</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>-1.2314</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:12">
+    <row r="7" s="1" customFormat="1" spans="1:13">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -2651,35 +2673,38 @@
       <c r="C7" s="1">
         <v>-1.23930495978553</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
+        <v>-1.17837362842636</v>
+      </c>
+      <c r="E7" s="3">
         <v>-0.527</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>-1.2514</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>-0.6043</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>-1.2532</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>-0.5491</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>-1.2406</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>-1.2399</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>-1.2435</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>-1.2398</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="1" spans="1:12">
+    <row r="8" s="1" customFormat="1" spans="1:13">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -2689,35 +2714,38 @@
       <c r="C8" s="1">
         <v>-1.23849222520113</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="1">
+        <v>-1.17716810025632</v>
+      </c>
+      <c r="E8" s="3">
         <v>-0.5223</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>-1.2608</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>-0.6047</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>-1.2652</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>-0.5479</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>-1.2456</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <v>-1.243</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>-1.2419</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>-1.2434</v>
       </c>
     </row>
-    <row r="9" s="1" customFormat="1" spans="1:12">
+    <row r="9" s="1" customFormat="1" spans="1:13">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -2727,35 +2755,38 @@
       <c r="C9" s="1">
         <v>-1.23335643431639</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="1">
+        <v>-1.17123672758763</v>
+      </c>
+      <c r="E9" s="3">
         <v>-0.5122</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>-1.2636</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>-0.6014</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>-1.27</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <v>-0.5424</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>-1.2443</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>-1.2405</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>-1.2337</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>-1.2414</v>
       </c>
     </row>
-    <row r="10" s="1" customFormat="1" spans="1:12">
+    <row r="10" s="1" customFormat="1" spans="1:13">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -2765,35 +2796,38 @@
       <c r="C10" s="1">
         <v>-1.22305026809653</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="1">
+        <v>-1.16048827566641</v>
+      </c>
+      <c r="E10" s="3">
         <v>-0.4957</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>-1.2584</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>-0.5936</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>-1.266</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <v>-0.5318</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>-1.2357</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>-1.2314</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>-1.2176</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>-1.2329</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" spans="1:12">
+    <row r="11" s="1" customFormat="1" spans="1:13">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -2803,35 +2837,38 @@
       <c r="C11" s="1">
         <v>-1.20699731903488</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="1">
+        <v>-1.14422256076764</v>
+      </c>
+      <c r="E11" s="3">
         <v>-0.4715</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>-1.2439</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>-0.5804</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>-1.2516</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <v>-0.5151</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>-1.2185</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>-1.2149</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>-1.1925</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>-1.2169</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" spans="1:12">
+    <row r="12" s="1" customFormat="1" spans="1:13">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -2841,35 +2878,38 @@
       <c r="C12" s="1">
         <v>-1.18415428954427</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="1">
+        <v>-1.12088579232613</v>
+      </c>
+      <c r="E12" s="3">
         <v>-0.4379</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>-1.2182</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>-0.5609</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>-1.2247</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="3">
         <v>-0.4912</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12" s="1">
         <v>-1.1915</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K12" s="1">
         <v>-1.1895</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>-1.1569</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>-1.1921</v>
       </c>
     </row>
-    <row r="13" s="1" customFormat="1" spans="1:12">
+    <row r="13" s="1" customFormat="1" spans="1:13">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -2879,35 +2919,38 @@
       <c r="C13" s="1">
         <v>-1.15414075067028</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="1">
+        <v>-1.09042360489482</v>
+      </c>
+      <c r="E13" s="3">
         <v>-0.3934</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>-1.1796</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>-0.534</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>-1.1832</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>-0.4588</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>-1.1531</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <v>-1.1541</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>-1.1092</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>-1.1572</v>
       </c>
     </row>
-    <row r="14" s="1" customFormat="1" spans="1:12">
+    <row r="14" s="1" customFormat="1" spans="1:13">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -2917,35 +2960,38 @@
       <c r="C14" s="1">
         <v>-1.11580965147456</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="1">
+        <v>-1.05176670656402</v>
+      </c>
+      <c r="E14" s="3">
         <v>-0.3357</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>-1.1258</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <v>-0.4983</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>-1.1243</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <v>-0.4165</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <v>-1.1017</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <v>-1.107</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>-1.0475</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>-1.1107</v>
       </c>
     </row>
-    <row r="15" s="1" customFormat="1" spans="1:12">
+    <row r="15" s="1" customFormat="1" spans="1:13">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -2955,35 +3001,38 @@
       <c r="C15" s="1">
         <v>-1.06820991957107</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="1">
+        <v>-1.00379164830943</v>
+      </c>
+      <c r="E15" s="3">
         <v>-0.2625</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>-1.0542</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="3">
         <v>-0.4524</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>-1.0449</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <v>-0.3625</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <v>-1.0353</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K15" s="1">
         <v>-1.0466</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>-0.9697</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>-1.0507</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" spans="1:12">
+    <row r="16" s="1" customFormat="1" spans="1:13">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -2993,31 +3042,34 @@
       <c r="C16" s="1">
         <v>-1.01007922252012</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="1">
+        <v>-0.945339399255005</v>
+      </c>
+      <c r="E16" s="3">
         <v>-0.171</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>-0.9622</v>
       </c>
-      <c r="F16" s="3">
+      <c r="G16" s="3">
         <v>-0.3943</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <v>-0.9414</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="3">
         <v>-0.2949</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>-0.9518</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K16" s="1">
         <v>-0.9708</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>-0.8734</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>-0.9754</v>
       </c>
     </row>

</xml_diff>

<commit_message>
collect data for VopX VopXfull
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -65,39 +65,6 @@
     </comment>
   </commentList>
 </comments>
-</file>
-
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="tmp" type="6" background="1" refreshedVersion="2" saveData="1">
-    <textPr sourceFile="/Users/yerong/Documents/William/tmp/tmp.txt">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="2" name="tmp1" type="6" background="1" refreshedVersion="2" saveData="1">
-    <textPr sourceFile="F:\William\tmp.txt">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="3" name="tmp_full" type="6" background="1" refreshedVersion="2" saveData="1">
-    <textPr sourceFile="F:\William\tmp_full.txt">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="4" name="tmp_single" type="6" background="1" refreshedVersion="2" saveData="1">
-    <textPr sourceFile="F:\William\tmp_single.txt">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -246,9 +213,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -261,23 +228,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -290,79 +241,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -381,9 +264,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -397,6 +295,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -404,8 +348,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -420,13 +387,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,55 +441,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -498,31 +471,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,7 +495,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -552,13 +531,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -570,31 +549,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -611,6 +578,78 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -631,39 +670,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -672,190 +678,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -933,46 +900,6 @@
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
-</file>
-
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
-    <queryTableFields count="1">
-      <queryTableField id="1" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
-    <queryTableFields count="1">
-      <queryTableField id="1" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
-    <queryTableFields count="1">
-      <queryTableField id="1" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_3" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
-    <queryTableFields count="1">
-      <queryTableField id="1" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2436,8 +2363,8 @@
   <sheetPr/>
   <dimension ref="A1:M16384"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -2526,16 +2453,16 @@
         <v>-0.5127</v>
       </c>
       <c r="J2" s="1">
-        <v>-1.0943</v>
+        <v>-1.0857</v>
       </c>
       <c r="K2" s="1">
-        <v>-1.1123</v>
+        <v>-1.1029</v>
       </c>
       <c r="L2" s="2">
         <v>-1.1812</v>
       </c>
       <c r="M2" s="2">
-        <v>-1.1089</v>
+        <v>-1.0998</v>
       </c>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:13">
@@ -2567,16 +2494,16 @@
         <v>-0.524</v>
       </c>
       <c r="J3" s="1">
-        <v>-1.1177</v>
+        <v>-1.1087</v>
       </c>
       <c r="K3" s="1">
-        <v>-1.1315</v>
+        <v>-1.1218</v>
       </c>
       <c r="L3" s="2">
         <v>-1.2007</v>
       </c>
       <c r="M3" s="2">
-        <v>-1.1286</v>
+        <v>-1.1193</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:13">
@@ -2608,16 +2535,16 @@
         <v>-0.5337</v>
       </c>
       <c r="J4" s="1">
-        <v>-1.1385</v>
+        <v>-1.1291</v>
       </c>
       <c r="K4" s="1">
-        <v>-1.1482</v>
+        <v>-1.1383</v>
       </c>
       <c r="L4" s="2">
         <v>-1.2173</v>
       </c>
       <c r="M4" s="2">
-        <v>-1.146</v>
+        <v>-1.1364</v>
       </c>
     </row>
     <row r="5" s="1" customFormat="1" spans="1:13">
@@ -2649,16 +2576,16 @@
         <v>-0.5414</v>
       </c>
       <c r="J5" s="1">
-        <v>-1.1562</v>
+        <v>-1.1465</v>
       </c>
       <c r="K5" s="1">
-        <v>-1.162</v>
+        <v>-1.152</v>
       </c>
       <c r="L5" s="2">
         <v>-1.2304</v>
       </c>
       <c r="M5" s="2">
-        <v>-1.1605</v>
+        <v>-1.1507</v>
       </c>
     </row>
     <row r="6" s="1" customFormat="1" spans="1:13">
@@ -2690,16 +2617,16 @@
         <v>-0.5467</v>
       </c>
       <c r="J6" s="1">
-        <v>-1.1702</v>
+        <v>-1.1602</v>
       </c>
       <c r="K6" s="1">
-        <v>-1.1725</v>
+        <v>-1.1623</v>
       </c>
       <c r="L6" s="2">
         <v>-1.2394</v>
       </c>
       <c r="M6" s="2">
-        <v>-1.1717</v>
+        <v>-1.1616</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:13">
@@ -2731,16 +2658,16 @@
         <v>-0.5491</v>
       </c>
       <c r="J7" s="1">
-        <v>-1.1798</v>
+        <v>-1.1695</v>
       </c>
       <c r="K7" s="1">
-        <v>-1.179</v>
+        <v>-1.1688</v>
       </c>
       <c r="L7" s="2">
         <v>-1.2435</v>
       </c>
       <c r="M7" s="2">
-        <v>-1.179</v>
+        <v>-1.1687</v>
       </c>
     </row>
     <row r="8" s="1" customFormat="1" spans="1:13">
@@ -2772,16 +2699,16 @@
         <v>-0.5479</v>
       </c>
       <c r="J8" s="1">
-        <v>-1.1841</v>
+        <v>-1.1736</v>
       </c>
       <c r="K8" s="1">
-        <v>-1.1809</v>
+        <v>-1.1706</v>
       </c>
       <c r="L8" s="2">
         <v>-1.2419</v>
       </c>
       <c r="M8" s="2">
-        <v>-1.1816</v>
+        <v>-1.1711</v>
       </c>
     </row>
     <row r="9" s="1" customFormat="1" spans="1:13">
@@ -2813,16 +2740,16 @@
         <v>-0.5424</v>
       </c>
       <c r="J9" s="1">
-        <v>-1.1823</v>
+        <v>-1.1716</v>
       </c>
       <c r="K9" s="1">
-        <v>-1.1774</v>
+        <v>-1.167</v>
       </c>
       <c r="L9" s="2">
         <v>-1.2337</v>
       </c>
       <c r="M9" s="2">
-        <v>-1.1787</v>
+        <v>-1.1682</v>
       </c>
     </row>
     <row r="10" s="1" customFormat="1" spans="1:13">
@@ -2854,16 +2781,16 @@
         <v>-0.5318</v>
       </c>
       <c r="J10" s="1">
-        <v>-1.1732</v>
+        <v>-1.1625</v>
       </c>
       <c r="K10" s="1">
-        <v>-1.1676</v>
+        <v>-1.1572</v>
       </c>
       <c r="L10" s="2">
         <v>-1.2176</v>
       </c>
       <c r="M10" s="2">
-        <v>-1.1695</v>
+        <v>-1.159</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="1" spans="1:13">
@@ -2895,16 +2822,16 @@
         <v>-0.5151</v>
       </c>
       <c r="J11" s="1">
-        <v>-1.1556</v>
+        <v>-1.145</v>
       </c>
       <c r="K11" s="1">
-        <v>-1.1505</v>
+        <v>-1.1403</v>
       </c>
       <c r="L11" s="2">
         <v>-1.1925</v>
       </c>
       <c r="M11" s="2">
-        <v>-1.153</v>
+        <v>-1.1425</v>
       </c>
     </row>
     <row r="12" s="1" customFormat="1" spans="1:13">
@@ -2936,16 +2863,16 @@
         <v>-0.4912</v>
       </c>
       <c r="J12" s="1">
-        <v>-1.1283</v>
+        <v>-1.1179</v>
       </c>
       <c r="K12" s="1">
-        <v>-1.1251</v>
+        <v>-1.115</v>
       </c>
       <c r="L12" s="2">
         <v>-1.1569</v>
       </c>
       <c r="M12" s="2">
-        <v>-1.128</v>
+        <v>-1.1176</v>
       </c>
     </row>
     <row r="13" s="1" customFormat="1" spans="1:13">
@@ -2977,16 +2904,16 @@
         <v>-0.4588</v>
       </c>
       <c r="J13" s="1">
-        <v>-1.0897</v>
+        <v>-1.0797</v>
       </c>
       <c r="K13" s="1">
-        <v>-1.0901</v>
+        <v>-1.0802</v>
       </c>
       <c r="L13" s="2">
         <v>-1.1092</v>
       </c>
       <c r="M13" s="2">
-        <v>-1.0931</v>
+        <v>-1.083</v>
       </c>
     </row>
     <row r="14" s="1" customFormat="1" spans="1:13">
@@ -3018,16 +2945,16 @@
         <v>-0.4165</v>
       </c>
       <c r="J14" s="1">
-        <v>-1.0381</v>
+        <v>-1.0286</v>
       </c>
       <c r="K14" s="1">
-        <v>-1.044</v>
+        <v>-1.0345</v>
       </c>
       <c r="L14" s="2">
         <v>-1.0475</v>
       </c>
       <c r="M14" s="2">
-        <v>-1.0468</v>
+        <v>-1.0372</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="1" spans="1:13">
@@ -3059,16 +2986,16 @@
         <v>-0.3625</v>
       </c>
       <c r="J15" s="1">
-        <v>-0.9716</v>
+        <v>-0.9629</v>
       </c>
       <c r="K15" s="1">
-        <v>-0.9853</v>
+        <v>-0.9763</v>
       </c>
       <c r="L15" s="2">
         <v>-0.9697</v>
       </c>
       <c r="M15" s="2">
-        <v>-0.9876</v>
+        <v>-0.9786</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="1" spans="1:13">
@@ -3100,16 +3027,16 @@
         <v>-0.2949</v>
       </c>
       <c r="J16" s="1">
-        <v>-0.8879</v>
+        <v>-0.8805</v>
       </c>
       <c r="K16" s="1">
-        <v>-0.9121</v>
+        <v>-0.9037</v>
       </c>
       <c r="L16" s="2">
         <v>-0.8734</v>
       </c>
       <c r="M16" s="2">
-        <v>-0.9133</v>
+        <v>-0.9052</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="1"/>

</xml_diff>

<commit_message>
precision plot for PBEnew and PBEhigh
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20145" windowHeight="7365" tabRatio="500" activeTab="3"/>
+    <workbookView windowWidth="20145" windowHeight="8400" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="data11" sheetId="1" r:id="rId1"/>
@@ -241,10 +241,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -256,17 +256,17 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -285,18 +285,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -309,44 +302,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -354,6 +333,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -383,16 +369,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -400,7 +386,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -415,7 +415,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,55 +439,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,7 +463,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -505,13 +559,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,43 +577,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -571,31 +589,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,25 +609,21 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -648,11 +644,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -672,32 +674,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -706,151 +682,175 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2391,7 +2391,7 @@
   <sheetPr/>
   <dimension ref="A1:M16384"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:M16"/>
     </sheetView>
   </sheetViews>
@@ -19448,17 +19448,17 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C2" sqref="C2:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="3" width="12.625"/>
-    <col min="4" max="4" width="15.75" customWidth="1"/>
-    <col min="5" max="5" width="13.75"/>
-    <col min="6" max="6" width="18.375" customWidth="1"/>
-    <col min="7" max="7" width="13.875" customWidth="1"/>
-    <col min="8" max="8" width="15.75" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
+    <col min="5" max="5" width="10.75" customWidth="1"/>
+    <col min="6" max="6" width="14.25" customWidth="1"/>
+    <col min="7" max="7" width="11.125" customWidth="1"/>
+    <col min="8" max="8" width="11.25" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="11" max="11" width="15.75" customWidth="1"/>
   </cols>
@@ -19513,22 +19513,23 @@
         <v>-9.34142444866186</v>
       </c>
       <c r="F2">
-        <v>-9.36272175</v>
+        <v>-9.36103175</v>
       </c>
       <c r="G2" s="1">
-        <v>0.0212973013381394</v>
+        <v>0.0207866660239055</v>
       </c>
       <c r="H2">
-        <v>-9.34142444866186</v>
+        <f t="shared" ref="H2:H16" si="0">F2+G2</f>
+        <v>-9.34024508397609</v>
       </c>
       <c r="I2">
-        <v>-9.36272175</v>
+        <v>-9.3677675</v>
       </c>
       <c r="J2" s="1">
-        <v>0.0212973013381394</v>
+        <v>0.0207866660239055</v>
       </c>
       <c r="K2">
-        <v>-9.34142444866186</v>
+        <v>-9.34698083397609</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -19548,22 +19549,23 @@
         <v>-9.34203116612822</v>
       </c>
       <c r="F3">
-        <v>-9.36334625</v>
+        <v>-9.361692</v>
       </c>
       <c r="G3" s="1">
-        <v>0.0213150838717795</v>
+        <v>0.020989686451872</v>
       </c>
       <c r="H3">
-        <v>-9.34203116612822</v>
+        <f t="shared" si="0"/>
+        <v>-9.34070231354813</v>
       </c>
       <c r="I3">
-        <v>-9.36334625</v>
+        <v>-9.368439</v>
       </c>
       <c r="J3" s="1">
-        <v>0.0213150838717795</v>
+        <v>0.020989686451872</v>
       </c>
       <c r="K3">
-        <v>-9.34203116612822</v>
+        <v>-9.34744931354813</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -19583,22 +19585,23 @@
         <v>-9.34252731341168</v>
       </c>
       <c r="F4">
-        <v>-9.36387875</v>
+        <v>-9.36226375</v>
       </c>
       <c r="G4" s="1">
-        <v>0.0213514365883235</v>
+        <v>0.0210678377004562</v>
       </c>
       <c r="H4">
-        <v>-9.34252731341168</v>
+        <f t="shared" si="0"/>
+        <v>-9.34119591229954</v>
       </c>
       <c r="I4">
-        <v>-9.36387875</v>
+        <v>-9.36901625</v>
       </c>
       <c r="J4" s="1">
-        <v>0.0213514365883235</v>
+        <v>0.0210678377004562</v>
       </c>
       <c r="K4">
-        <v>-9.34252731341168</v>
+        <v>-9.34794841229954</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -19618,22 +19621,23 @@
         <v>-9.34292050564871</v>
       </c>
       <c r="F5">
-        <v>-9.364291</v>
+        <v>-9.362721</v>
       </c>
       <c r="G5" s="1">
-        <v>0.0213704943512894</v>
+        <v>0.0211449184301374</v>
       </c>
       <c r="H5">
-        <v>-9.34292050564871</v>
+        <f t="shared" si="0"/>
+        <v>-9.34157608156986</v>
       </c>
       <c r="I5">
-        <v>-9.364291</v>
+        <v>-9.3694765</v>
       </c>
       <c r="J5" s="1">
-        <v>0.0213704943512894</v>
+        <v>0.0211449184301374</v>
       </c>
       <c r="K5">
-        <v>-9.34292050564871</v>
+        <v>-9.34833158156986</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -19653,22 +19657,23 @@
         <v>-9.34319526886993</v>
       </c>
       <c r="F6">
-        <v>-9.36458075</v>
+        <v>-9.36304625</v>
       </c>
       <c r="G6" s="1">
-        <v>0.0213854811300705</v>
+        <v>0.0211876360212808</v>
       </c>
       <c r="H6">
-        <v>-9.34319526886993</v>
+        <f t="shared" si="0"/>
+        <v>-9.34185861397872</v>
       </c>
       <c r="I6">
-        <v>-9.36458075</v>
+        <v>-9.3698085</v>
       </c>
       <c r="J6" s="1">
-        <v>0.0213854811300705</v>
+        <v>0.0211876360212808</v>
       </c>
       <c r="K6">
-        <v>-9.34319526886993</v>
+        <v>-9.34862086397872</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -19688,22 +19693,23 @@
         <v>-9.34329465155856</v>
       </c>
       <c r="F7">
-        <v>-9.36471925</v>
+        <v>-9.3632295</v>
       </c>
       <c r="G7" s="1">
-        <v>0.0214245984414376</v>
+        <v>0.0212305313736267</v>
       </c>
       <c r="H7">
-        <v>-9.34329465155856</v>
+        <f t="shared" si="0"/>
+        <v>-9.34199896862637</v>
       </c>
       <c r="I7">
-        <v>-9.36471925</v>
+        <v>-9.36999225</v>
       </c>
       <c r="J7" s="1">
-        <v>0.0214245984414376</v>
+        <v>0.0212305313736267</v>
       </c>
       <c r="K7">
-        <v>-9.34329465155856</v>
+        <v>-9.34876171862637</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -19723,22 +19729,23 @@
         <v>-9.34324236527863</v>
       </c>
       <c r="F8">
-        <v>-9.364684</v>
+        <v>-9.363235</v>
       </c>
       <c r="G8" s="1">
-        <v>0.0214416347213709</v>
+        <v>0.0212778746105494</v>
       </c>
       <c r="H8">
-        <v>-9.34324236527863</v>
+        <f t="shared" si="0"/>
+        <v>-9.34195712538945</v>
       </c>
       <c r="I8">
-        <v>-9.364684</v>
+        <v>-9.3700015</v>
       </c>
       <c r="J8" s="1">
-        <v>0.0214416347213709</v>
+        <v>0.0212778746105494</v>
       </c>
       <c r="K8">
-        <v>-9.34324236527863</v>
+        <v>-9.34872362538945</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -19758,22 +19765,23 @@
         <v>-9.34298510923149</v>
       </c>
       <c r="F9">
-        <v>-9.36446125</v>
+        <v>-9.36305075</v>
       </c>
       <c r="G9" s="1">
-        <v>0.0214761407685137</v>
+        <v>0.0213136945617403</v>
       </c>
       <c r="H9">
-        <v>-9.34298510923149</v>
+        <f t="shared" si="0"/>
+        <v>-9.34173705543826</v>
       </c>
       <c r="I9">
-        <v>-9.36446125</v>
+        <v>-9.36981575</v>
       </c>
       <c r="J9" s="1">
-        <v>0.0214761407685137</v>
+        <v>0.0213136945617403</v>
       </c>
       <c r="K9">
-        <v>-9.34298510923149</v>
+        <v>-9.34850205543826</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -19793,22 +19801,23 @@
         <v>-9.3425189263749</v>
       </c>
       <c r="F10">
-        <v>-9.36401425</v>
+        <v>-9.3626495</v>
       </c>
       <c r="G10" s="1">
-        <v>0.0214953236250955</v>
+        <v>0.0213480337310196</v>
       </c>
       <c r="H10">
-        <v>-9.3425189263749</v>
+        <f t="shared" si="0"/>
+        <v>-9.34130146626898</v>
       </c>
       <c r="I10">
-        <v>-9.36401425</v>
+        <v>-9.3694085</v>
       </c>
       <c r="J10" s="1">
-        <v>0.0214953236250955</v>
+        <v>0.0213480337310196</v>
       </c>
       <c r="K10">
-        <v>-9.3425189263749</v>
+        <v>-9.34806046626898</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -19828,22 +19837,23 @@
         <v>-9.34181344827522</v>
       </c>
       <c r="F11">
-        <v>-9.363318</v>
+        <v>-9.3619875</v>
       </c>
       <c r="G11" s="1">
-        <v>0.0215045517247771</v>
+        <v>0.021378424677586</v>
       </c>
       <c r="H11">
-        <v>-9.34181344827522</v>
+        <f t="shared" si="0"/>
+        <v>-9.34060907532241</v>
       </c>
       <c r="I11">
-        <v>-9.363318</v>
+        <v>-9.36874575</v>
       </c>
       <c r="J11" s="1">
-        <v>0.0215045517247771</v>
+        <v>0.021378424677586</v>
       </c>
       <c r="K11">
-        <v>-9.34181344827522</v>
+        <v>-9.34736732532241</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -19863,22 +19873,23 @@
         <v>-9.34080128378352</v>
       </c>
       <c r="F12">
-        <v>-9.36232725</v>
+        <v>-9.36103725</v>
       </c>
       <c r="G12" s="1">
-        <v>0.0215259662164836</v>
+        <v>0.0214031006727538</v>
       </c>
       <c r="H12">
-        <v>-9.34080128378352</v>
+        <f t="shared" si="0"/>
+        <v>-9.33963414932725</v>
       </c>
       <c r="I12">
-        <v>-9.36232725</v>
+        <v>-9.36779125</v>
       </c>
       <c r="J12" s="1">
-        <v>0.0215259662164836</v>
+        <v>0.0214031006727538</v>
       </c>
       <c r="K12">
-        <v>-9.34080128378352</v>
+        <v>-9.34638814932725</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -19898,22 +19909,23 @@
         <v>-9.33948007495655</v>
       </c>
       <c r="F13">
-        <v>-9.3610255</v>
+        <v>-9.3597695</v>
       </c>
       <c r="G13" s="1">
-        <v>0.0215454250434452</v>
+        <v>0.0214281307651274</v>
       </c>
       <c r="H13">
-        <v>-9.33948007495655</v>
+        <f t="shared" si="0"/>
+        <v>-9.33834136923487</v>
       </c>
       <c r="I13">
-        <v>-9.3610255</v>
+        <v>-9.3665155</v>
       </c>
       <c r="J13" s="1">
-        <v>0.0215454250434452</v>
+        <v>0.0214281307651274</v>
       </c>
       <c r="K13">
-        <v>-9.33948007495655</v>
+        <v>-9.34508736923487</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -19933,22 +19945,23 @@
         <v>-9.33780344436616</v>
       </c>
       <c r="F14">
-        <v>-9.359363</v>
+        <v>-9.35814475</v>
       </c>
       <c r="G14" s="1">
-        <v>0.02155955563384</v>
+        <v>0.0214509041842186</v>
       </c>
       <c r="H14">
-        <v>-9.33780344436616</v>
+        <f t="shared" si="0"/>
+        <v>-9.33669384581578</v>
       </c>
       <c r="I14">
-        <v>-9.359363</v>
+        <v>-9.3648825</v>
       </c>
       <c r="J14" s="1">
-        <v>0.02155955563384</v>
+        <v>0.0214509041842186</v>
       </c>
       <c r="K14">
-        <v>-9.33780344436616</v>
+        <v>-9.34343159581578</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -19968,22 +19981,23 @@
         <v>-9.33572266567675</v>
       </c>
       <c r="F15">
-        <v>-9.3572985</v>
+        <v>-9.35611575</v>
       </c>
       <c r="G15" s="1">
-        <v>0.0215758343232551</v>
+        <v>0.0214703613916357</v>
       </c>
       <c r="H15">
-        <v>-9.33572266567675</v>
+        <f t="shared" si="0"/>
+        <v>-9.33464538860837</v>
       </c>
       <c r="I15">
-        <v>-9.3572985</v>
+        <v>-9.36283875</v>
       </c>
       <c r="J15" s="1">
-        <v>0.0215758343232551</v>
+        <v>0.0214703613916357</v>
       </c>
       <c r="K15">
-        <v>-9.33572266567675</v>
+        <v>-9.34136838860836</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -20003,22 +20017,23 @@
         <v>-9.33318746929334</v>
       </c>
       <c r="F16">
-        <v>-9.35477725</v>
+        <v>-9.3536185</v>
       </c>
       <c r="G16" s="1">
-        <v>0.0215897807066604</v>
+        <v>0.0214884013356759</v>
       </c>
       <c r="H16">
-        <v>-9.33318746929334</v>
+        <f t="shared" si="0"/>
+        <v>-9.33213009866432</v>
       </c>
       <c r="I16">
-        <v>-9.35477725</v>
+        <v>-9.360343</v>
       </c>
       <c r="J16" s="1">
-        <v>0.0215897807066604</v>
+        <v>0.0214884013356759</v>
       </c>
       <c r="K16">
-        <v>-9.33318746929334</v>
+        <v>-9.33885459866432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct data for shift
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -24,6 +24,9 @@
     <definedName name="ExternalData_1" localSheetId="2">CCmd!$M$2:$M$16</definedName>
     <definedName name="ExternalData_2" localSheetId="2">CCmd!$K$2:$K$16</definedName>
     <definedName name="ExternalData_3" localSheetId="2">CCmd!$J$2:$J$16</definedName>
+    <definedName name="res" localSheetId="4">shift!$D$2:$D$16</definedName>
+    <definedName name="res_1" localSheetId="4">shift!$E$2:$E$16</definedName>
+    <definedName name="res_2" localSheetId="4">shift!$F$2:$F$16</definedName>
     <definedName name="tmp" localSheetId="2">CCmd!$L$2:$L$16</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
@@ -82,6 +85,32 @@
     </comment>
   </commentList>
 </comments>
+</file>
+
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="res" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/yerong/Documents/William/res.txt">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="res1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/yerong/Documents/William/res.txt">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="res2" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/yerong/Documents/William/res.txt">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -268,7 +297,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -280,6 +312,13 @@
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -302,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -322,6 +361,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -334,6 +381,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19449,321 +19508,321 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <v>7.0226732791159003</v>
-      </c>
-      <c r="C2">
-        <v>-1.1639764723508701</v>
-      </c>
-      <c r="D2">
-        <v>-1.1173999999999999</v>
-      </c>
-      <c r="E2">
-        <v>-1.1563000000000001</v>
-      </c>
-      <c r="F2">
-        <v>-1.1416999999999999</v>
+      <c r="B2" s="12">
+        <v>7.0226730000000002</v>
+      </c>
+      <c r="C2" s="9">
+        <v>-1.1639764720000001</v>
+      </c>
+      <c r="D2" s="9">
+        <v>-1.1201000000000001</v>
+      </c>
+      <c r="E2" s="9">
+        <v>-1.1343000000000001</v>
+      </c>
+      <c r="F2" s="9">
+        <v>-1.1306</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
-        <v>6.9563557718344402</v>
-      </c>
-      <c r="C3">
-        <v>-1.17477787803332</v>
-      </c>
-      <c r="D3">
-        <v>-1.1415</v>
-      </c>
-      <c r="E3">
-        <v>-1.1737</v>
-      </c>
-      <c r="F3">
-        <v>-1.1604000000000001</v>
+      <c r="B3" s="12">
+        <v>6.9563560000000004</v>
+      </c>
+      <c r="C3" s="9">
+        <v>-1.174777878</v>
+      </c>
+      <c r="D3" s="9">
+        <v>-1.1435999999999999</v>
+      </c>
+      <c r="E3" s="9">
+        <v>-1.1559999999999999</v>
+      </c>
+      <c r="F3" s="9">
+        <v>-1.1534</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
-        <v>6.8900382645529898</v>
-      </c>
-      <c r="C4">
-        <v>-1.1862852487092499</v>
-      </c>
-      <c r="D4">
-        <v>-1.163</v>
-      </c>
-      <c r="E4">
-        <v>-1.1874</v>
-      </c>
-      <c r="F4">
-        <v>-1.1760999999999999</v>
+      <c r="B4" s="12">
+        <v>6.8900379999999997</v>
+      </c>
+      <c r="C4" s="9">
+        <v>-1.186285249</v>
+      </c>
+      <c r="D4" s="9">
+        <v>-1.1645000000000001</v>
+      </c>
+      <c r="E4" s="9">
+        <v>-1.1732</v>
+      </c>
+      <c r="F4" s="9">
+        <v>-1.1712</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
-        <v>6.8237207572715297</v>
-      </c>
-      <c r="C5">
-        <v>-1.19511971445925</v>
-      </c>
-      <c r="D5">
-        <v>-1.1814</v>
-      </c>
-      <c r="E5">
-        <v>-1.1980999999999999</v>
-      </c>
-      <c r="F5">
-        <v>-1.1892</v>
+      <c r="B5" s="12">
+        <v>6.8237209999999999</v>
+      </c>
+      <c r="C5" s="9">
+        <v>-1.1951197140000001</v>
+      </c>
+      <c r="D5" s="9">
+        <v>-1.1823999999999999</v>
+      </c>
+      <c r="E5" s="9">
+        <v>-1.1875</v>
+      </c>
+      <c r="F5" s="9">
+        <v>-1.1861999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B6">
-        <v>6.7574032499900696</v>
-      </c>
-      <c r="C6">
-        <v>-1.2017894965402101</v>
-      </c>
-      <c r="D6">
-        <v>-1.1960999999999999</v>
-      </c>
-      <c r="E6">
-        <v>-1.2051000000000001</v>
-      </c>
-      <c r="F6">
-        <v>-1.1991000000000001</v>
+      <c r="B6" s="12">
+        <v>6.757403</v>
+      </c>
+      <c r="C6" s="9">
+        <v>-1.201789497</v>
+      </c>
+      <c r="D6" s="9">
+        <v>-1.1964999999999999</v>
+      </c>
+      <c r="E6" s="9">
+        <v>-1.1984999999999999</v>
+      </c>
+      <c r="F6" s="9">
+        <v>-1.1978</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B7">
-        <v>6.6910857427086103</v>
-      </c>
-      <c r="C7">
-        <v>-1.2050370835905799</v>
-      </c>
-      <c r="D7">
-        <v>-1.2062999999999999</v>
-      </c>
-      <c r="E7">
-        <v>-1.208</v>
-      </c>
-      <c r="F7">
-        <v>-1.2053</v>
+      <c r="B7" s="12">
+        <v>6.6910860000000003</v>
+      </c>
+      <c r="C7" s="9">
+        <v>-1.205037084</v>
+      </c>
+      <c r="D7" s="9">
+        <v>-1.2061999999999999</v>
+      </c>
+      <c r="E7" s="9">
+        <v>-1.2055</v>
+      </c>
+      <c r="F7" s="9">
+        <v>-1.2055</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B8">
-        <v>6.62476823542716</v>
-      </c>
-      <c r="C8">
-        <v>-1.2041587944819701</v>
-      </c>
-      <c r="D8">
-        <v>-1.2112000000000001</v>
-      </c>
-      <c r="E8">
-        <v>-1.2059</v>
-      </c>
-      <c r="F8">
-        <v>-1.2071000000000001</v>
+      <c r="B8" s="12">
+        <v>6.6247680000000004</v>
+      </c>
+      <c r="C8" s="9">
+        <v>-1.204158794</v>
+      </c>
+      <c r="D8" s="9">
+        <v>-1.2107000000000001</v>
+      </c>
+      <c r="E8" s="9">
+        <v>-1.2079</v>
+      </c>
+      <c r="F8" s="9">
+        <v>-1.2084999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B9">
-        <v>6.5584507281456998</v>
-      </c>
-      <c r="C9">
-        <v>-1.1990502111569299</v>
-      </c>
-      <c r="D9">
-        <v>-1.2099</v>
-      </c>
-      <c r="E9">
-        <v>-1.1980999999999999</v>
-      </c>
-      <c r="F9">
-        <v>-1.204</v>
+      <c r="B9" s="12">
+        <v>6.5584509999999998</v>
+      </c>
+      <c r="C9" s="9">
+        <v>-1.1990502110000001</v>
+      </c>
+      <c r="D9" s="9">
+        <v>-1.2091000000000001</v>
+      </c>
+      <c r="E9" s="9">
+        <v>-1.2049000000000001</v>
+      </c>
+      <c r="F9" s="9">
+        <v>-1.2060999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B10">
-        <v>6.4921332208642397</v>
-      </c>
-      <c r="C10">
-        <v>-1.1888687986748601</v>
-      </c>
-      <c r="D10">
-        <v>-1.2013</v>
-      </c>
-      <c r="E10">
-        <v>-1.1837</v>
-      </c>
-      <c r="F10">
-        <v>-1.1949000000000001</v>
+      <c r="B10" s="12">
+        <v>6.4921329999999999</v>
+      </c>
+      <c r="C10" s="9">
+        <v>-1.188868799</v>
+      </c>
+      <c r="D10" s="9">
+        <v>-1.2003999999999999</v>
+      </c>
+      <c r="E10" s="9">
+        <v>-1.1956</v>
+      </c>
+      <c r="F10" s="9">
+        <v>-1.1974</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B11">
-        <v>6.4258157135827902</v>
-      </c>
-      <c r="C11">
-        <v>-1.17288753288264</v>
-      </c>
-      <c r="D11">
-        <v>-1.1842999999999999</v>
-      </c>
-      <c r="E11">
-        <v>-1.1615</v>
-      </c>
-      <c r="F11">
+      <c r="B11" s="12">
+        <v>6.4258160000000002</v>
+      </c>
+      <c r="C11" s="9">
+        <v>-1.1728875329999999</v>
+      </c>
+      <c r="D11" s="9">
+        <v>-1.1833</v>
+      </c>
+      <c r="E11" s="9">
         <v>-1.1791</v>
+      </c>
+      <c r="F11" s="9">
+        <v>-1.1814</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B12">
-        <v>6.3594982063013301</v>
-      </c>
-      <c r="C12">
-        <v>-1.15031135712294</v>
-      </c>
-      <c r="D12">
-        <v>-1.1575</v>
-      </c>
-      <c r="E12">
-        <v>-1.1305000000000001</v>
-      </c>
-      <c r="F12">
-        <v>-1.1553</v>
+      <c r="B12" s="12">
+        <v>6.3594980000000003</v>
+      </c>
+      <c r="C12" s="9">
+        <v>-1.1503113570000001</v>
+      </c>
+      <c r="D12" s="9">
+        <v>-1.1567000000000001</v>
+      </c>
+      <c r="E12" s="9">
+        <v>-1.1543000000000001</v>
+      </c>
+      <c r="F12" s="9">
+        <v>-1.1569</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B13">
-        <v>6.29318069901987</v>
-      </c>
-      <c r="C13">
-        <v>-1.1203201807302301</v>
-      </c>
-      <c r="D13">
-        <v>-1.1193</v>
-      </c>
-      <c r="E13">
-        <v>-1.0891999999999999</v>
-      </c>
-      <c r="F13">
-        <v>-1.1225000000000001</v>
+      <c r="B13" s="12">
+        <v>6.2931809999999997</v>
+      </c>
+      <c r="C13" s="9">
+        <v>-1.1203201810000001</v>
+      </c>
+      <c r="D13" s="9">
+        <v>-1.119</v>
+      </c>
+      <c r="E13" s="9">
+        <v>-1.1197999999999999</v>
+      </c>
+      <c r="F13" s="9">
+        <v>-1.1226</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B14">
-        <v>6.2268631917384099</v>
-      </c>
-      <c r="C14">
-        <v>-1.0821441716037701</v>
-      </c>
-      <c r="D14">
-        <v>-1.0682</v>
-      </c>
-      <c r="E14">
-        <v>-1.0361</v>
-      </c>
-      <c r="F14">
-        <v>-1.0790999999999999</v>
+      <c r="B14" s="12">
+        <v>6.2268629999999998</v>
+      </c>
+      <c r="C14" s="9">
+        <v>-1.082144172</v>
+      </c>
+      <c r="D14" s="9">
+        <v>-1.0686</v>
+      </c>
+      <c r="E14" s="9">
+        <v>-1.0744</v>
+      </c>
+      <c r="F14" s="9">
+        <v>-1.077</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B15">
-        <v>6.1605456844569604</v>
-      </c>
-      <c r="C15">
-        <v>-1.03457424671424</v>
-      </c>
-      <c r="D15">
-        <v>-1.0022</v>
-      </c>
-      <c r="E15">
-        <v>-0.96930000000000005</v>
-      </c>
-      <c r="F15">
-        <v>-1.0236000000000001</v>
+      <c r="B15" s="12">
+        <v>6.1605460000000001</v>
+      </c>
+      <c r="C15" s="9">
+        <v>-1.0345742469999999</v>
+      </c>
+      <c r="D15" s="9">
+        <v>-1.0038</v>
+      </c>
+      <c r="E15" s="9">
+        <v>-1.0162</v>
+      </c>
+      <c r="F15" s="9">
+        <v>-1.0184</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B16">
-        <v>6.0942281771755002</v>
-      </c>
-      <c r="C16">
-        <v>-0.97661555095345398</v>
-      </c>
-      <c r="D16">
-        <v>-0.91910000000000003</v>
-      </c>
-      <c r="E16">
-        <v>-0.88690000000000002</v>
-      </c>
-      <c r="F16">
-        <v>-0.95420000000000005</v>
+      <c r="B16" s="12">
+        <v>6.0942280000000002</v>
+      </c>
+      <c r="C16" s="9">
+        <v>-0.97661555099999997</v>
+      </c>
+      <c r="D16" s="9">
+        <v>-0.92230000000000001</v>
+      </c>
+      <c r="E16" s="9">
+        <v>-0.94359999999999999</v>
+      </c>
+      <c r="F16" s="9">
+        <v>-0.94489999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the up and down data
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="460" windowWidth="24320" windowHeight="15540" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="1280" yWindow="460" windowWidth="24320" windowHeight="15540" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="data11" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,15 @@
     <definedName name="ExternalData_1" localSheetId="2">CCmd!$M$2:$M$16</definedName>
     <definedName name="ExternalData_2" localSheetId="2">CCmd!$K$2:$K$16</definedName>
     <definedName name="ExternalData_3" localSheetId="2">CCmd!$J$2:$J$16</definedName>
+    <definedName name="res" localSheetId="5">down!$C$2:$C$16</definedName>
     <definedName name="res" localSheetId="4">shift!$D$2:$D$16</definedName>
+    <definedName name="res" localSheetId="6">up!$C$2:$C$16</definedName>
+    <definedName name="res_1" localSheetId="5">down!$D$2:$D$16</definedName>
     <definedName name="res_1" localSheetId="4">shift!$E$2:$E$16</definedName>
+    <definedName name="res_1" localSheetId="6">up!$E$2:$E$16</definedName>
+    <definedName name="res_2" localSheetId="5">down!$E$2:$E$16</definedName>
     <definedName name="res_2" localSheetId="4">shift!$F$2:$F$16</definedName>
+    <definedName name="res_2" localSheetId="6">up!$D$2:$D$16</definedName>
     <definedName name="tmp" localSheetId="2">CCmd!$L$2:$L$16</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
@@ -110,11 +116,53 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="4" name="res3" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/yerong/Documents/William/res.txt">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="res4" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/yerong/Documents/William/res.txt">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="res5" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/yerong/Documents/William/res.txt">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" name="res6" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/yerong/Documents/William/res.txt">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="8" name="res7" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/yerong/Documents/William/res.txt">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="9" name="res8" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/yerong/Documents/William/res.txt">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="60">
   <si>
     <t>C(A)</t>
   </si>
@@ -292,13 +340,16 @@
   <si>
     <t>VopXfull</t>
   </si>
+  <si>
+    <t>QM+phn</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -368,7 +419,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,15 +435,39 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19501,7 +19576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F16"/>
     </sheetView>
   </sheetViews>
@@ -19832,136 +19907,286 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="A1:E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>7.0959732791159</v>
       </c>
+      <c r="C2">
+        <v>-1.6639764720000001</v>
+      </c>
+      <c r="D2">
+        <v>-1.5972999999999999</v>
+      </c>
+      <c r="E2">
+        <v>-1.5455000000000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2">
         <v>7.0296557718344399</v>
       </c>
+      <c r="C3">
+        <v>-1.674777878</v>
+      </c>
+      <c r="D3">
+        <v>-1.6272</v>
+      </c>
+      <c r="E3">
+        <v>-1.5806</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3">
         <v>6.9633382645529904</v>
       </c>
+      <c r="C4">
+        <v>-1.686285249</v>
+      </c>
+      <c r="D4">
+        <v>-1.6536999999999999</v>
+      </c>
+      <c r="E4">
+        <v>-1.6138999999999999</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3">
         <v>6.8970207572715303</v>
       </c>
+      <c r="C5">
+        <v>-1.6951197140000001</v>
+      </c>
+      <c r="D5">
+        <v>-1.6763999999999999</v>
+      </c>
+      <c r="E5">
+        <v>-1.6448</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="3">
         <v>6.8307032499900702</v>
       </c>
+      <c r="C6">
+        <v>-1.701789497</v>
+      </c>
+      <c r="D6">
+        <v>-1.6943999999999999</v>
+      </c>
+      <c r="E6">
+        <v>-1.6729000000000001</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="3">
         <v>6.76438574270861</v>
       </c>
+      <c r="C7">
+        <v>-1.705037084</v>
+      </c>
+      <c r="D7">
+        <v>-1.7070000000000001</v>
+      </c>
+      <c r="E7">
+        <v>-1.6975</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2">
         <v>6.6980682354271597</v>
       </c>
+      <c r="C8">
+        <v>-1.704158794</v>
+      </c>
+      <c r="D8">
+        <v>-1.7133</v>
+      </c>
+      <c r="E8">
+        <v>-1.718</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="3">
         <v>6.6317507281457004</v>
       </c>
+      <c r="C9">
+        <v>-1.6990502110000001</v>
+      </c>
+      <c r="D9">
+        <v>-1.7124999999999999</v>
+      </c>
+      <c r="E9">
+        <v>-1.7337</v>
+      </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="3">
         <v>6.5654332208642403</v>
       </c>
+      <c r="C10">
+        <v>-1.688868799</v>
+      </c>
+      <c r="D10">
+        <v>-1.7033</v>
+      </c>
+      <c r="E10">
+        <v>-1.7437</v>
+      </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="3">
         <v>6.4991157135827899</v>
       </c>
+      <c r="C11">
+        <v>-1.6728875329999999</v>
+      </c>
+      <c r="D11">
+        <v>-1.6847000000000001</v>
+      </c>
+      <c r="E11">
+        <v>-1.7470000000000001</v>
+      </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="3">
         <v>6.4327982063013298</v>
       </c>
+      <c r="C12">
+        <v>-1.6503113570000001</v>
+      </c>
+      <c r="D12">
+        <v>-1.6553</v>
+      </c>
+      <c r="E12">
+        <v>-1.7423999999999999</v>
+      </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="3">
         <v>6.3664806990198697</v>
       </c>
+      <c r="C13">
+        <v>-1.6203201810000001</v>
+      </c>
+      <c r="D13">
+        <v>-1.6135999999999999</v>
+      </c>
+      <c r="E13">
+        <v>-1.7287999999999999</v>
+      </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="3">
         <v>6.3001631917384104</v>
       </c>
+      <c r="C14">
+        <v>-1.582144172</v>
+      </c>
+      <c r="D14">
+        <v>-1.5582</v>
+      </c>
+      <c r="E14">
+        <v>-1.7047000000000001</v>
+      </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="2">
         <v>6.2338456844569601</v>
       </c>
+      <c r="C15">
+        <v>-1.5345742469999999</v>
+      </c>
+      <c r="D15">
+        <v>-1.4871000000000001</v>
+      </c>
+      <c r="E15">
+        <v>-1.6684000000000001</v>
+      </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="2">
         <v>6.1675281771754999</v>
+      </c>
+      <c r="C16">
+        <v>-1.4766155510000001</v>
+      </c>
+      <c r="D16">
+        <v>-1.3984000000000001</v>
+      </c>
+      <c r="E16">
+        <v>-1.6181000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -19971,138 +20196,286 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B16"/>
+      <selection activeCell="E16" sqref="A1:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>7.0959732791159</v>
       </c>
+      <c r="C2">
+        <v>-0.66397647199999998</v>
+      </c>
+      <c r="D2">
+        <v>-0.64229999999999998</v>
+      </c>
+      <c r="E2">
+        <v>-0.72870000000000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2">
         <v>7.0296557718344399</v>
       </c>
+      <c r="C3">
+        <v>-0.674777878</v>
+      </c>
+      <c r="D3">
+        <v>-0.65920000000000001</v>
+      </c>
+      <c r="E3">
+        <v>-0.73270000000000002</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3">
         <v>6.9633382645529904</v>
       </c>
+      <c r="C4">
+        <v>-0.68628524899999999</v>
+      </c>
+      <c r="D4">
+        <v>-0.67449999999999999</v>
+      </c>
+      <c r="E4">
+        <v>-0.73370000000000002</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="3">
         <v>6.8970207572715303</v>
       </c>
+      <c r="C5">
+        <v>-0.69511971400000006</v>
+      </c>
+      <c r="D5">
+        <v>-0.68769999999999998</v>
+      </c>
+      <c r="E5">
+        <v>-0.73119999999999996</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="3">
         <v>6.8307032499900702</v>
       </c>
+      <c r="C6">
+        <v>-0.70178949700000004</v>
+      </c>
+      <c r="D6">
+        <v>-0.69820000000000004</v>
+      </c>
+      <c r="E6">
+        <v>-0.72470000000000001</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="3">
         <v>6.76438574270861</v>
       </c>
+      <c r="C7">
+        <v>-0.70503708399999998</v>
+      </c>
+      <c r="D7">
+        <v>-0.70550000000000002</v>
+      </c>
+      <c r="E7">
+        <v>-0.71360000000000001</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2">
         <v>6.6980682354271597</v>
       </c>
+      <c r="C8">
+        <v>-0.70415879400000003</v>
+      </c>
+      <c r="D8">
+        <v>-0.7087</v>
+      </c>
+      <c r="E8">
+        <v>-0.69710000000000005</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="3">
         <v>6.6317507281457004</v>
       </c>
+      <c r="C9">
+        <v>-0.69905021099999998</v>
+      </c>
+      <c r="D9">
+        <v>-0.70699999999999996</v>
+      </c>
+      <c r="E9">
+        <v>-0.67449999999999999</v>
+      </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="3">
         <v>6.5654332208642403</v>
       </c>
+      <c r="C10">
+        <v>-0.68886879899999998</v>
+      </c>
+      <c r="D10">
+        <v>-0.69920000000000004</v>
+      </c>
+      <c r="E10">
+        <v>-0.64490000000000003</v>
+      </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="3">
         <v>6.4991157135827899</v>
       </c>
+      <c r="C11">
+        <v>-0.67288753300000004</v>
+      </c>
+      <c r="D11">
+        <v>-0.68410000000000004</v>
+      </c>
+      <c r="E11">
+        <v>-0.60719999999999996</v>
+      </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="3">
         <v>6.4327982063013298</v>
       </c>
+      <c r="C12">
+        <v>-0.65031135699999998</v>
+      </c>
+      <c r="D12">
+        <v>-0.6603</v>
+      </c>
+      <c r="E12">
+        <v>-0.56040000000000001</v>
+      </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="3">
         <v>6.3664806990198697</v>
       </c>
+      <c r="C13">
+        <v>-0.62032018099999997</v>
+      </c>
+      <c r="D13">
+        <v>-0.62609999999999999</v>
+      </c>
+      <c r="E13">
+        <v>-0.50309999999999999</v>
+      </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="3">
         <v>6.3001631917384104</v>
       </c>
+      <c r="C14">
+        <v>-0.58214417200000002</v>
+      </c>
+      <c r="D14">
+        <v>-0.5796</v>
+      </c>
+      <c r="E14">
+        <v>-0.43390000000000001</v>
+      </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="2">
         <v>6.2338456844569601</v>
       </c>
+      <c r="C15">
+        <v>-0.534574247</v>
+      </c>
+      <c r="D15">
+        <v>-0.51829999999999998</v>
+      </c>
+      <c r="E15">
+        <v>-0.35120000000000001</v>
+      </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="2">
         <v>6.1675281771754999</v>
+      </c>
+      <c r="C16">
+        <v>-0.47661555100000003</v>
+      </c>
+      <c r="D16">
+        <v>-0.43969999999999998</v>
+      </c>
+      <c r="E16">
+        <v>-0.25309999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify X6 extreme weight
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="7950" tabRatio="500" activeTab="2"/>
+    <workbookView windowWidth="20385" windowHeight="7950" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="data11" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62">
   <si>
     <t>C(A)</t>
   </si>
@@ -363,6 +363,9 @@
     <t>VopXfull</t>
   </si>
   <si>
+    <t>opt</t>
+  </si>
+  <si>
     <t>QM+phn</t>
   </si>
 </sst>
@@ -371,14 +374,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.000000"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.000000"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -393,8 +404,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -404,34 +414,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -446,7 +435,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -454,9 +443,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -468,24 +457,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -501,6 +496,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -508,14 +518,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -530,23 +540,16 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -561,7 +564,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -573,175 +744,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -752,6 +755,63 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -787,63 +847,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -855,13 +858,13 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -873,134 +876,134 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1011,14 +1014,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1027,16 +1028,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
@@ -1096,8 +1096,8 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_6" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp_1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
     </queryTableFields>
@@ -1106,7 +1106,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -1116,7 +1116,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -1136,7 +1136,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -1146,6 +1146,16 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_4" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
+    <queryTableFields count="1">
+      <queryTableField id="1" dataBound="0"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_5" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
     <queryTableFields count="1">
@@ -1155,8 +1165,8 @@
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_4" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_6" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -1165,18 +1175,8 @@
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp_1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
-    <queryTableFields count="1">
-      <queryTableField id="1" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -1196,7 +1196,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -1206,7 +1206,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -1512,111 +1512,111 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="16">
+      <c r="A2" s="15">
         <v>7.734603659</v>
       </c>
       <c r="B2">
         <v>-9.29974075</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="15">
         <f t="shared" ref="C2:C25" si="0">B2+E2</f>
         <v>-9.27877112419782</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="16">
         <v>0</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="15">
         <v>0.0209696258021805</v>
       </c>
-      <c r="I2" s="16"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="16">
+      <c r="A3" s="15">
         <v>7.398316544</v>
       </c>
       <c r="B3">
         <v>-9.303271</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="15">
         <f t="shared" si="0"/>
         <v>-9.28217704928256</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <v>0</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="15">
         <v>0.0210939507174438</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="16">
+      <c r="A4" s="15">
         <v>7.06202942799999</v>
       </c>
       <c r="B4">
         <v>-9.305298</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <f t="shared" si="0"/>
         <v>-9.28401399136472</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <v>0</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="15">
         <v>0.0212840086352783</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="16">
+      <c r="A5" s="15">
         <v>6.99477200493787</v>
       </c>
       <c r="B5">
         <v>-9.30541825</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <f t="shared" si="0"/>
         <v>-9.28414069068237</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="16">
         <v>0</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="15">
         <v>0.0212775593176295</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>6.92751458181347</v>
       </c>
       <c r="B6">
         <v>-9.305416</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="15">
         <f t="shared" si="0"/>
         <v>-9.305416</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>0</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="16">
+      <c r="A7" s="15">
         <v>6.86025715868907</v>
       </c>
       <c r="B7">
         <v>-9.305258</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="15">
         <f t="shared" si="0"/>
         <v>-9.28394005617462</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <v>0</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="15">
         <v>0.0213179438253818</v>
       </c>
     </row>
@@ -1627,11 +1627,11 @@
       <c r="B8">
         <v>-9.30494375</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="15">
         <f t="shared" si="0"/>
         <v>-9.28360454025992</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>0</v>
       </c>
       <c r="E8">
@@ -1639,308 +1639,308 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="16">
+      <c r="A9" s="15">
         <v>6.72574231244026</v>
       </c>
       <c r="B9">
         <v>-9.30443575</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="15">
         <f t="shared" si="0"/>
         <v>-9.28085089283634</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>0</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="15">
         <v>0.0235848571636644</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="16">
+      <c r="A10" s="15">
         <v>6.65848488931586</v>
       </c>
       <c r="B10">
         <v>-9.303711</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="15">
         <f t="shared" si="0"/>
         <v>-9.303711</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="16">
         <v>0</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="16">
+      <c r="A11" s="15">
         <v>6.59122746619145</v>
       </c>
       <c r="B11">
         <v>-9.3027445</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="15">
         <f t="shared" si="0"/>
         <v>-9.3027445</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <v>0</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="16">
+      <c r="A12" s="15">
         <v>6.52397004306705</v>
       </c>
       <c r="B12">
         <v>-9.30149675</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="15">
         <f t="shared" si="0"/>
         <v>-9.30149675</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <v>0</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="16">
+      <c r="A13" s="15">
         <v>6.45671261994265</v>
       </c>
       <c r="B13">
         <v>-9.29993175</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="15">
         <f t="shared" si="0"/>
         <v>-9.29993175</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="16">
         <v>0</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="16">
+      <c r="A14" s="15">
         <v>6.389455197</v>
       </c>
       <c r="B14">
         <v>-9.2980065</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="15">
         <f t="shared" si="0"/>
         <v>-9.2765447062902</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="16">
         <v>0</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E14" s="15">
         <v>0.0214617937098034</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="16">
+      <c r="A15" s="15">
         <v>6.05316808099999</v>
       </c>
       <c r="B15">
         <v>-9.281312</v>
       </c>
-      <c r="C15" s="16">
+      <c r="C15" s="15">
         <f t="shared" si="0"/>
         <v>-9.25981534941733</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="16">
         <v>0</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="15">
         <v>0.0214966505826721</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="16">
+      <c r="A16" s="15">
         <v>5.71688096599999</v>
       </c>
       <c r="B16">
         <v>-9.24699775</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="15">
         <f t="shared" si="0"/>
         <v>-9.22545581578752</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="16">
         <v>0</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="15">
         <v>0.0215419342124851</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="16">
+      <c r="A17" s="15">
         <v>5.38059385</v>
       </c>
       <c r="B17">
         <v>-9.18425575</v>
       </c>
-      <c r="C17" s="16">
+      <c r="C17" s="15">
         <f t="shared" si="0"/>
         <v>-9.16266257845306</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="16">
         <v>0</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="15">
         <v>0.0215931715469442</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="16">
+      <c r="A18" s="15">
         <v>5.044306734</v>
       </c>
       <c r="B18">
         <v>-9.07655725</v>
       </c>
-      <c r="C18" s="16">
+      <c r="C18" s="15">
         <f t="shared" si="0"/>
         <v>-9.05490492455843</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="16">
         <v>0</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="15">
         <v>0.0216523254415718</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="16">
+      <c r="A19" s="15">
         <v>4.70801961899999</v>
       </c>
       <c r="B19">
         <v>-8.89676175</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C19" s="15">
         <f t="shared" si="0"/>
         <v>-8.87509644543177</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="16">
         <v>0</v>
       </c>
-      <c r="E19" s="16">
+      <c r="E19" s="15">
         <v>0.0216653045682302</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="16">
+      <c r="A20" s="15">
         <v>4.37173250299999</v>
       </c>
       <c r="B20">
         <v>-8.610972</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="15">
         <f t="shared" si="0"/>
         <v>-8.58969112874629</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="16">
         <v>0</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="15">
         <v>0.021280871253706</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="16">
+      <c r="A21" s="15">
         <v>4.035445387</v>
       </c>
       <c r="B21">
         <v>-8.184804</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="15">
         <f t="shared" si="0"/>
         <v>-8.1644223392305</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="16">
         <v>0</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="15">
         <v>0.0203816607694967</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="16">
+      <c r="A22" s="15">
         <v>3.69915827100001</v>
       </c>
       <c r="B22">
         <v>-7.561232</v>
       </c>
-      <c r="C22" s="16">
+      <c r="C22" s="15">
         <f t="shared" si="0"/>
         <v>-7.54245840350752</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="16">
         <v>0</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="15">
         <v>0.0187735964924786</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="16">
+      <c r="A23" s="15">
         <v>3.36287115500002</v>
       </c>
       <c r="B23">
         <v>-6.6218255</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="15">
         <f t="shared" si="0"/>
         <v>-6.60562327498075</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="16">
         <v>0</v>
       </c>
-      <c r="E23" s="16">
+      <c r="E23" s="15">
         <v>0.0162022250192528</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="16">
+      <c r="A24" s="15">
         <v>3.02658403900003</v>
       </c>
       <c r="B24">
         <v>-5.380071</v>
       </c>
-      <c r="C24" s="16">
+      <c r="C24" s="15">
         <f t="shared" si="0"/>
         <v>-5.36397948973004</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="16">
         <v>0</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="15">
         <v>0.0160915102699602</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="16">
+      <c r="A25" s="15">
         <v>2.69029692300004</v>
       </c>
       <c r="B25">
         <v>-3.654861</v>
       </c>
-      <c r="C25" s="16">
+      <c r="C25" s="15">
         <f t="shared" si="0"/>
         <v>-3.63930487592718</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="16">
         <v>0</v>
       </c>
-      <c r="E25" s="16">
+      <c r="E25" s="15">
         <v>0.0155561240728216</v>
       </c>
     </row>
@@ -1951,28 +1951,28 @@
       <c r="D29" s="8"/>
     </row>
     <row r="30" spans="4:4">
-      <c r="D30" s="17"/>
+      <c r="D30" s="16"/>
     </row>
     <row r="31" spans="4:4">
-      <c r="D31" s="17"/>
+      <c r="D31" s="16"/>
     </row>
     <row r="32" spans="4:4">
-      <c r="D32" s="17"/>
+      <c r="D32" s="16"/>
     </row>
     <row r="33" spans="4:4">
-      <c r="D33" s="17"/>
+      <c r="D33" s="16"/>
     </row>
     <row r="34" spans="4:4">
-      <c r="D34" s="17"/>
+      <c r="D34" s="16"/>
     </row>
     <row r="35" spans="4:4">
-      <c r="D35" s="17"/>
+      <c r="D35" s="16"/>
     </row>
     <row r="36" spans="4:4">
-      <c r="D36" s="17"/>
+      <c r="D36" s="16"/>
     </row>
     <row r="37" spans="4:4">
-      <c r="D37" s="17"/>
+      <c r="D37" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2018,20 +2018,20 @@
       </c>
     </row>
     <row r="2" spans="2:7">
-      <c r="B2" s="16">
+      <c r="B2" s="15">
         <v>7.62651333736756</v>
       </c>
       <c r="C2">
         <v>-9.35571075</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="16">
         <f t="shared" ref="D2:D29" si="0">C2+F2</f>
         <v>-9.35571075</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="16">
         <v>0</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="15">
         <v>0</v>
       </c>
       <c r="G2">
@@ -2039,20 +2039,20 @@
       </c>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="16">
+      <c r="B3" s="15">
         <v>7.29492580096027</v>
       </c>
       <c r="C3">
         <v>-9.36041425</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <f t="shared" si="0"/>
         <v>-9.36041425</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <v>0</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="15">
         <v>0</v>
       </c>
       <c r="G3">
@@ -2069,11 +2069,11 @@
       <c r="C4">
         <v>-9.36272175</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <f t="shared" si="0"/>
         <v>-9.34142444866186</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <v>-1.74798</v>
       </c>
       <c r="F4" s="8">
@@ -2093,11 +2093,11 @@
       <c r="C5">
         <v>-9.36334625</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="16">
         <f t="shared" si="0"/>
         <v>-9.34203116612822</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="16">
         <v>-1.37949</v>
       </c>
       <c r="F5" s="8">
@@ -2111,17 +2111,17 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="15">
         <v>6.96333826455299</v>
       </c>
       <c r="C6">
         <v>-9.36387875</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <f t="shared" si="0"/>
         <v>-9.34252731341168</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <v>-0.649711</v>
       </c>
       <c r="F6" s="8">
@@ -2135,17 +2135,17 @@
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="15">
         <v>6.89702075727153</v>
       </c>
       <c r="C7">
         <v>-9.364291</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <f t="shared" si="0"/>
         <v>-9.34292050564871</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <v>-0.436941</v>
       </c>
       <c r="F7" s="8">
@@ -2159,17 +2159,17 @@
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="15">
         <v>6.83070324999007</v>
       </c>
       <c r="C8">
         <v>-9.36458075</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <f t="shared" si="0"/>
         <v>-9.34319526886993</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="16">
         <v>-0.194466</v>
       </c>
       <c r="F8" s="8">
@@ -2183,17 +2183,17 @@
       <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="15">
         <v>6.76438574270861</v>
       </c>
       <c r="C9">
         <v>-9.36471925</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <f t="shared" si="0"/>
         <v>-9.34329465155856</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="16">
         <v>0.083872</v>
       </c>
       <c r="F9" s="8">
@@ -2213,11 +2213,11 @@
       <c r="C10">
         <v>-9.364684</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="16">
         <f t="shared" si="0"/>
         <v>-9.34324236527863</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="16">
         <v>0.40474</v>
       </c>
       <c r="F10" s="8">
@@ -2231,17 +2231,17 @@
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="15">
         <v>6.6317507281457</v>
       </c>
       <c r="C11">
         <v>-9.36446125</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <f t="shared" si="0"/>
         <v>-9.34298510923149</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="16">
         <v>0.766066</v>
       </c>
       <c r="F11" s="8">
@@ -2255,17 +2255,17 @@
       <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="15">
         <v>6.56543322086424</v>
       </c>
       <c r="C12">
         <v>-9.36401425</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <f t="shared" si="0"/>
         <v>-9.3425189263749</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="16">
         <v>1.209655</v>
       </c>
       <c r="F12" s="8">
@@ -2279,17 +2279,17 @@
       <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="15">
         <v>6.49911571358279</v>
       </c>
       <c r="C13">
         <v>-9.363318</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="16">
         <f t="shared" si="0"/>
         <v>-9.34181344827522</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="16">
         <v>1.650845</v>
       </c>
       <c r="F13" s="8">
@@ -2303,17 +2303,17 @@
       <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="15">
         <v>6.43279820630133</v>
       </c>
       <c r="C14">
         <v>-9.36232725</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="16">
         <f t="shared" si="0"/>
         <v>-9.34080128378352</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="16">
         <v>2.184954</v>
       </c>
       <c r="F14" s="8">
@@ -2327,17 +2327,17 @@
       <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="15">
         <v>6.36648069901987</v>
       </c>
       <c r="C15">
         <v>-9.3610255</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="16">
         <f t="shared" si="0"/>
         <v>-9.33948007495655</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="16">
         <v>2.81936</v>
       </c>
       <c r="F15" s="8">
@@ -2351,17 +2351,17 @@
       <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="15">
         <v>6.30016319173841</v>
       </c>
       <c r="C16">
         <v>-9.359363</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="16">
         <f t="shared" si="0"/>
         <v>-9.33780344436616</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="16">
         <v>3.470399</v>
       </c>
       <c r="F16" s="8">
@@ -2381,11 +2381,11 @@
       <c r="C17">
         <v>-9.3572985</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="16">
         <f t="shared" si="0"/>
         <v>-9.33572266567675</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="16">
         <v>8.313759</v>
       </c>
       <c r="F17" s="8">
@@ -2405,11 +2405,11 @@
       <c r="C18">
         <v>-9.35477725</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="16">
         <f t="shared" si="0"/>
         <v>-9.33318746929334</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="16">
         <v>16.364584</v>
       </c>
       <c r="F18" s="8">
@@ -2423,17 +2423,17 @@
       <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="15">
         <v>5.96857565533113</v>
       </c>
       <c r="C19">
         <v>-9.3439195</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="16">
         <f t="shared" si="0"/>
         <v>-9.3439195</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="16">
         <v>29.162834</v>
       </c>
       <c r="F19">
@@ -2444,17 +2444,17 @@
       <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="15">
         <v>5.63698811892385</v>
       </c>
       <c r="C20">
         <v>-9.31057675</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="16">
         <f t="shared" si="0"/>
         <v>-9.31057675</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="16">
         <v>49.590418</v>
       </c>
       <c r="F20">
@@ -2465,17 +2465,17 @@
       <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="15">
         <v>5.30540058251656</v>
       </c>
       <c r="C21">
         <v>-9.2470915</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="16">
         <f t="shared" si="0"/>
         <v>-9.2470915</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="16">
         <v>81.795232</v>
       </c>
       <c r="F21">
@@ -2486,17 +2486,17 @@
       <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="15">
         <v>4.97381304610928</v>
       </c>
       <c r="C22">
         <v>-9.13348925</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="16">
         <f t="shared" si="0"/>
         <v>-9.13348925</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="16">
         <v>126.264436</v>
       </c>
       <c r="F22">
@@ -2507,17 +2507,17 @@
       <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="16">
+      <c r="B23" s="15">
         <v>4.64222550970199</v>
       </c>
       <c r="C23">
         <v>-8.9380785</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="16">
         <f t="shared" si="0"/>
         <v>-8.9380785</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="16">
         <v>184.537527</v>
       </c>
       <c r="F23">
@@ -2528,17 +2528,17 @@
       <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="16">
+      <c r="B24" s="15">
         <v>4.31063797329471</v>
       </c>
       <c r="C24">
         <v>-8.63161825</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="16">
         <f t="shared" si="0"/>
         <v>-8.63161825</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="16">
         <v>278.177108</v>
       </c>
       <c r="F24">
@@ -2549,17 +2549,17 @@
       <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="15">
         <v>3.97905043688742</v>
       </c>
       <c r="C25">
         <v>-8.18573275</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="16">
         <f t="shared" si="0"/>
         <v>-8.18573275</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="16">
         <v>410.94174</v>
       </c>
       <c r="F25">
@@ -2570,13 +2570,13 @@
       <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="16">
+      <c r="B26" s="15">
         <v>3.64746290048014</v>
       </c>
       <c r="C26">
         <v>-7.534209</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="16">
         <f t="shared" si="0"/>
         <v>-7.534209</v>
       </c>
@@ -2591,13 +2591,13 @@
       <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="16">
+      <c r="B27" s="15">
         <v>3.31587536407285</v>
       </c>
       <c r="C27">
         <v>-6.56529875</v>
       </c>
-      <c r="D27" s="17">
+      <c r="D27" s="16">
         <f t="shared" si="0"/>
         <v>-6.56529875</v>
       </c>
@@ -2612,20 +2612,20 @@
       <c r="A28" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="16">
         <v>2.98428782766557</v>
       </c>
       <c r="C28">
         <v>-5.3080285</v>
       </c>
-      <c r="D28" s="17">
+      <c r="D28" s="16">
         <f t="shared" si="0"/>
         <v>-5.3080285</v>
       </c>
       <c r="E28" s="8">
         <v>0</v>
       </c>
-      <c r="F28" s="17">
+      <c r="F28" s="16">
         <v>0</v>
       </c>
     </row>
@@ -2633,46 +2633,46 @@
       <c r="A29" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="16">
         <v>2.65270029125828</v>
       </c>
       <c r="C29">
         <v>-3.53590775</v>
       </c>
-      <c r="D29" s="17">
+      <c r="D29" s="16">
         <f t="shared" si="0"/>
         <v>-3.53590775</v>
       </c>
       <c r="E29" s="8">
         <v>0</v>
       </c>
-      <c r="F29" s="17">
+      <c r="F29" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="5:5">
-      <c r="E30" s="17"/>
+      <c r="E30" s="16"/>
     </row>
     <row r="31" spans="5:5">
-      <c r="E31" s="17"/>
+      <c r="E31" s="16"/>
     </row>
     <row r="32" spans="5:5">
-      <c r="E32" s="17"/>
+      <c r="E32" s="16"/>
     </row>
     <row r="33" spans="5:5">
-      <c r="E33" s="17"/>
+      <c r="E33" s="16"/>
     </row>
     <row r="34" spans="5:5">
-      <c r="E34" s="17"/>
+      <c r="E34" s="16"/>
     </row>
     <row r="35" spans="5:5">
-      <c r="E35" s="17"/>
+      <c r="E35" s="16"/>
     </row>
     <row r="36" spans="5:5">
-      <c r="E36" s="17"/>
+      <c r="E36" s="16"/>
     </row>
     <row r="37" spans="5:5">
-      <c r="E37" s="17"/>
+      <c r="E37" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -2686,8 +2686,8 @@
   <sheetPr/>
   <dimension ref="A1:M16384"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -2699,7 +2699,7 @@
     <col min="6" max="6" width="13.1666666666667" customWidth="1"/>
     <col min="7" max="7" width="10.3333333333333" customWidth="1"/>
     <col min="8" max="8" width="11.6666666666667" customWidth="1"/>
-    <col min="9" max="9" width="9.16666666666667" customWidth="1"/>
+    <col min="9" max="9" width="12.875" customWidth="1"/>
     <col min="10" max="10" width="12.1666666666667" customWidth="1"/>
     <col min="11" max="11" width="13.5" customWidth="1"/>
     <col min="12" max="12" width="11.8333333333333" customWidth="1"/>
@@ -2772,16 +2772,16 @@
       <c r="H2" s="10">
         <v>-0.5127</v>
       </c>
-      <c r="I2" s="15">
-        <v>-1.1061</v>
-      </c>
-      <c r="J2" s="15">
+      <c r="I2" s="5">
+        <v>-1.16397647235087</v>
+      </c>
+      <c r="J2" s="5">
         <v>-1.1251</v>
       </c>
       <c r="K2" s="14">
         <v>-1.1812</v>
       </c>
-      <c r="L2" s="15">
+      <c r="L2" s="5">
         <v>-1.1203</v>
       </c>
       <c r="M2">
@@ -2813,16 +2813,16 @@
       <c r="H3" s="10">
         <v>-0.524</v>
       </c>
-      <c r="I3" s="15">
-        <v>-1.1303</v>
-      </c>
-      <c r="J3" s="15">
+      <c r="I3" s="5">
+        <v>-1.17477787803301</v>
+      </c>
+      <c r="J3" s="5">
         <v>-1.1475</v>
       </c>
       <c r="K3" s="14">
         <v>-1.2007</v>
       </c>
-      <c r="L3" s="15">
+      <c r="L3" s="5">
         <v>-1.1438</v>
       </c>
       <c r="M3">
@@ -2854,16 +2854,16 @@
       <c r="H4" s="10">
         <v>-0.5337</v>
       </c>
-      <c r="I4" s="15">
-        <v>-1.1521</v>
-      </c>
-      <c r="J4" s="15">
+      <c r="I4" s="5">
+        <v>-1.186285248709</v>
+      </c>
+      <c r="J4" s="5">
         <v>-1.1654</v>
       </c>
       <c r="K4" s="14">
         <v>-1.2173</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="5">
         <v>-1.1623</v>
       </c>
       <c r="M4">
@@ -2895,16 +2895,16 @@
       <c r="H5" s="10">
         <v>-0.5414</v>
       </c>
-      <c r="I5" s="15">
-        <v>-1.171</v>
-      </c>
-      <c r="J5" s="15">
+      <c r="I5" s="5">
+        <v>-1.195119714459</v>
+      </c>
+      <c r="J5" s="5">
         <v>-1.1805</v>
       </c>
       <c r="K5" s="14">
         <v>-1.2304</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="5">
         <v>-1.1781</v>
       </c>
       <c r="M5">
@@ -2936,16 +2936,16 @@
       <c r="H6" s="10">
         <v>-0.5467</v>
       </c>
-      <c r="I6" s="15">
-        <v>-1.1864</v>
-      </c>
-      <c r="J6" s="15">
+      <c r="I6" s="5">
+        <v>-1.20178949653999</v>
+      </c>
+      <c r="J6" s="5">
         <v>-1.1924</v>
       </c>
       <c r="K6" s="14">
         <v>-1.2394</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="5">
         <v>-1.1906</v>
       </c>
       <c r="M6">
@@ -2977,16 +2977,16 @@
       <c r="H7" s="10">
         <v>-0.5491</v>
       </c>
-      <c r="I7" s="15">
-        <v>-1.2085</v>
-      </c>
-      <c r="J7" s="15">
+      <c r="I7" s="5">
+        <v>-1.20503708359101</v>
+      </c>
+      <c r="J7" s="5">
         <v>-1.2074</v>
       </c>
       <c r="K7" s="14">
         <v>-1.2435</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="5">
         <v>-1.2074</v>
       </c>
       <c r="M7">
@@ -3018,16 +3018,16 @@
       <c r="H8" s="10">
         <v>0</v>
       </c>
-      <c r="I8" s="15">
-        <v>-1.2068</v>
-      </c>
-      <c r="J8" s="15">
+      <c r="I8" s="5">
+        <v>-1.20522788652559</v>
+      </c>
+      <c r="J8" s="5">
         <v>-1.2059</v>
       </c>
       <c r="K8" s="14">
         <v>0</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="5">
         <v>-1.2059</v>
       </c>
       <c r="M8">
@@ -3059,16 +3059,16 @@
       <c r="H9" s="10">
         <v>-0.5479</v>
       </c>
-      <c r="I9" s="15">
-        <v>-1.204</v>
-      </c>
-      <c r="J9" s="15">
+      <c r="I9" s="5">
+        <v>-1.20415879448197</v>
+      </c>
+      <c r="J9" s="5">
         <v>-1.204</v>
       </c>
       <c r="K9" s="14">
         <v>-1.2419</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9" s="5">
         <v>-1.2038</v>
       </c>
       <c r="M9">
@@ -3100,16 +3100,16 @@
       <c r="H10" s="10">
         <v>-0.5424</v>
       </c>
-      <c r="I10" s="15">
-        <v>-1.2045</v>
-      </c>
-      <c r="J10" s="15">
+      <c r="I10" s="5">
+        <v>-1.19905021115693</v>
+      </c>
+      <c r="J10" s="5">
         <v>-1.2024</v>
       </c>
       <c r="K10" s="14">
         <v>-1.2337</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10" s="5">
         <v>-1.2029</v>
       </c>
       <c r="M10">
@@ -3141,16 +3141,16 @@
       <c r="H11" s="10">
         <v>-0.5318</v>
       </c>
-      <c r="I11" s="15">
-        <v>-1.1981</v>
-      </c>
-      <c r="J11" s="15">
+      <c r="I11" s="5">
+        <v>-1.18886879867486</v>
+      </c>
+      <c r="J11" s="5">
         <v>-1.1946</v>
       </c>
       <c r="K11" s="14">
         <v>-1.2176</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="5">
         <v>-1.1959</v>
       </c>
       <c r="M11">
@@ -3182,16 +3182,16 @@
       <c r="H12" s="10">
         <v>-0.5151</v>
       </c>
-      <c r="I12" s="15">
-        <v>-1.1641</v>
-      </c>
-      <c r="J12" s="15">
+      <c r="I12" s="5">
+        <v>-1.17288753288264</v>
+      </c>
+      <c r="J12" s="5">
         <v>-1.16</v>
       </c>
       <c r="K12" s="14">
         <v>-1.1925</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="5">
         <v>-1.1626</v>
       </c>
       <c r="M12">
@@ -3223,16 +3223,16 @@
       <c r="H13" s="10">
         <v>-0.4912</v>
       </c>
-      <c r="I13" s="15">
-        <v>-1.1605</v>
-      </c>
-      <c r="J13" s="15">
+      <c r="I13" s="5">
+        <v>-1.15031135712294</v>
+      </c>
+      <c r="J13" s="5">
         <v>-1.157</v>
       </c>
       <c r="K13" s="14">
         <v>-1.1569</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="5">
         <v>-1.1595</v>
       </c>
       <c r="M13">
@@ -3264,16 +3264,16 @@
       <c r="H14" s="10">
         <v>-0.4588</v>
       </c>
-      <c r="I14" s="15">
-        <v>-1.1265</v>
-      </c>
-      <c r="J14" s="15">
+      <c r="I14" s="5">
+        <v>-1.12032018073023</v>
+      </c>
+      <c r="J14" s="5">
         <v>-1.1249</v>
       </c>
       <c r="K14" s="14">
         <v>-1.1092</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L14" s="5">
         <v>-1.1277</v>
       </c>
       <c r="M14">
@@ -3305,16 +3305,16 @@
       <c r="H15" s="10">
         <v>-0.4165</v>
       </c>
-      <c r="I15" s="15">
-        <v>-1.0804</v>
-      </c>
-      <c r="J15" s="15">
+      <c r="I15" s="5">
+        <v>-1.08214417160377</v>
+      </c>
+      <c r="J15" s="5">
         <v>-1.082</v>
       </c>
       <c r="K15" s="14">
         <v>-1.0475</v>
       </c>
-      <c r="L15" s="15">
+      <c r="L15" s="5">
         <v>-1.085</v>
       </c>
       <c r="M15">
@@ -3346,16 +3346,16 @@
       <c r="H16" s="10">
         <v>-0.3625</v>
       </c>
-      <c r="I16" s="15">
-        <v>-1.0203</v>
-      </c>
-      <c r="J16" s="15">
+      <c r="I16" s="5">
+        <v>-1.03457424671424</v>
+      </c>
+      <c r="J16" s="5">
         <v>-1.0268</v>
       </c>
       <c r="K16" s="14">
         <v>-0.9697</v>
       </c>
-      <c r="L16" s="15">
+      <c r="L16" s="5">
         <v>-1.0298</v>
       </c>
       <c r="M16">
@@ -3387,16 +3387,16 @@
       <c r="H17" s="10">
         <v>-0.2949</v>
       </c>
-      <c r="I17" s="15">
-        <v>-0.9442</v>
-      </c>
-      <c r="J17" s="15">
+      <c r="I17" s="5">
+        <v>-0.976615550953454</v>
+      </c>
+      <c r="J17" s="5">
         <v>-0.9575</v>
       </c>
       <c r="K17" s="14">
         <v>-0.8734</v>
       </c>
-      <c r="L17" s="15">
+      <c r="L17" s="5">
         <v>-0.9601</v>
       </c>
     </row>
@@ -53103,329 +53103,349 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7">
-        <v>7.022673</v>
-      </c>
-      <c r="C2" s="5">
-        <v>-1.163976472</v>
+      <c r="B2" s="4">
+        <v>7.0226732791159</v>
+      </c>
+      <c r="C2">
+        <v>-1.16397647235087</v>
       </c>
       <c r="D2" s="5">
-        <v>-1.1201</v>
-      </c>
-      <c r="E2" s="5">
+        <v>-1.115</v>
+      </c>
+      <c r="E2" s="6">
         <v>-1.1343</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2">
         <v>-1.1306</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7">
-        <v>6.956356</v>
-      </c>
-      <c r="C3" s="5">
-        <v>-1.174777878</v>
+      <c r="B3" s="4">
+        <v>6.95635577183444</v>
+      </c>
+      <c r="C3">
+        <v>-1.17477787803301</v>
       </c>
       <c r="D3" s="5">
-        <v>-1.1436</v>
-      </c>
-      <c r="E3" s="5">
+        <v>-1.1388</v>
+      </c>
+      <c r="E3" s="6">
         <v>-1.156</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3">
         <v>-1.1534</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7">
-        <v>6.890038</v>
-      </c>
-      <c r="C4" s="5">
-        <v>-1.186285249</v>
+      <c r="B4" s="4">
+        <v>6.89003826455299</v>
+      </c>
+      <c r="C4">
+        <v>-1.186285248709</v>
       </c>
       <c r="D4" s="5">
-        <v>-1.1645</v>
-      </c>
-      <c r="E4" s="5">
+        <v>-1.1602</v>
+      </c>
+      <c r="E4" s="6">
         <v>-1.1732</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4">
         <v>-1.1712</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="7">
-        <v>6.823721</v>
-      </c>
-      <c r="C5" s="5">
-        <v>-1.195119714</v>
+      <c r="B5" s="4">
+        <v>6.82372075727153</v>
+      </c>
+      <c r="C5">
+        <v>-1.195119714459</v>
       </c>
       <c r="D5" s="5">
-        <v>-1.1824</v>
-      </c>
-      <c r="E5" s="5">
+        <v>-1.1787</v>
+      </c>
+      <c r="E5" s="6">
         <v>-1.1875</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5">
         <v>-1.1862</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="7">
-        <v>6.757403</v>
-      </c>
-      <c r="C6" s="5">
-        <v>-1.201789497</v>
+      <c r="B6" s="4">
+        <v>6.75740324999007</v>
+      </c>
+      <c r="C6">
+        <v>-1.20178949653999</v>
       </c>
       <c r="D6" s="5">
-        <v>-1.1965</v>
-      </c>
-      <c r="E6" s="5">
+        <v>-1.1936</v>
+      </c>
+      <c r="E6" s="6">
         <v>-1.1985</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6">
         <v>-1.1978</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="7">
-        <v>6.691086</v>
-      </c>
-      <c r="C7" s="5">
-        <v>-1.205037084</v>
+      <c r="B7" s="4">
+        <v>6.69108574270861</v>
+      </c>
+      <c r="C7">
+        <v>-1.20503708359101</v>
       </c>
       <c r="D7" s="5">
-        <v>-1.2062</v>
-      </c>
-      <c r="E7" s="5">
+        <v>-1.2043</v>
+      </c>
+      <c r="E7" s="6">
         <v>-1.2055</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7">
         <v>-1.2055</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="7">
+        <v>6.7454</v>
+      </c>
+      <c r="C8">
+        <v>-1.20522788652559</v>
+      </c>
+      <c r="D8" s="5">
+        <v>-1.2065</v>
+      </c>
+      <c r="E8" s="5">
+        <v>-1.2065</v>
+      </c>
+      <c r="F8" s="5">
+        <v>-1.2065</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="7">
-        <v>6.624768</v>
-      </c>
-      <c r="C8" s="5">
-        <v>-1.204158794</v>
-      </c>
-      <c r="D8" s="5">
-        <v>-1.2107</v>
-      </c>
-      <c r="E8" s="5">
-        <v>-1.2079</v>
-      </c>
-      <c r="F8" s="5">
+      <c r="B9" s="4">
+        <v>6.62476823542716</v>
+      </c>
+      <c r="C9">
+        <v>-1.20415879448197</v>
+      </c>
+      <c r="D9" s="5">
+        <v>-1.21</v>
+      </c>
+      <c r="E9" s="6">
+        <v>-1.2049</v>
+      </c>
+      <c r="F9">
         <v>-1.2085</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="7">
-        <v>6.558451</v>
-      </c>
-      <c r="C9" s="5">
-        <v>-1.199050211</v>
-      </c>
-      <c r="D9" s="5">
-        <v>-1.2091</v>
-      </c>
-      <c r="E9" s="5">
-        <v>-1.2049</v>
-      </c>
-      <c r="F9" s="5">
+      <c r="B10" s="4">
+        <v>6.5584507281457</v>
+      </c>
+      <c r="C10">
+        <v>-1.19905021115693</v>
+      </c>
+      <c r="D10" s="5">
+        <v>-1.2099</v>
+      </c>
+      <c r="E10" s="6">
+        <v>-1.1956</v>
+      </c>
+      <c r="F10">
         <v>-1.2061</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="4" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="7">
-        <v>6.492133</v>
-      </c>
-      <c r="C10" s="5">
-        <v>-1.188868799</v>
-      </c>
-      <c r="D10" s="5">
-        <v>-1.2004</v>
-      </c>
-      <c r="E10" s="5">
-        <v>-1.1956</v>
-      </c>
-      <c r="F10" s="5">
+      <c r="B11" s="4">
+        <v>6.49213322086424</v>
+      </c>
+      <c r="C11">
+        <v>-1.18886879867486</v>
+      </c>
+      <c r="D11" s="5">
+        <v>-1.203</v>
+      </c>
+      <c r="E11" s="6">
+        <v>-1.1791</v>
+      </c>
+      <c r="F11">
         <v>-1.1974</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="4" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="7">
-        <v>6.425816</v>
-      </c>
-      <c r="C11" s="5">
-        <v>-1.172887533</v>
-      </c>
-      <c r="D11" s="5">
-        <v>-1.1833</v>
-      </c>
-      <c r="E11" s="5">
-        <v>-1.1791</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="B12" s="4">
+        <v>6.42581571358279</v>
+      </c>
+      <c r="C12">
+        <v>-1.17288753288264</v>
+      </c>
+      <c r="D12" s="5">
+        <v>-1.1881</v>
+      </c>
+      <c r="E12" s="6">
+        <v>-1.1543</v>
+      </c>
+      <c r="F12">
         <v>-1.1814</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="4" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="7">
-        <v>6.359498</v>
-      </c>
-      <c r="C12" s="5">
-        <v>-1.150311357</v>
-      </c>
-      <c r="D12" s="5">
-        <v>-1.1567</v>
-      </c>
-      <c r="E12" s="5">
-        <v>-1.1543</v>
-      </c>
-      <c r="F12" s="5">
+      <c r="B13" s="4">
+        <v>6.35949820630133</v>
+      </c>
+      <c r="C13">
+        <v>-1.15031135712294</v>
+      </c>
+      <c r="D13" s="5">
+        <v>-1.1641</v>
+      </c>
+      <c r="E13" s="6">
+        <v>-1.1198</v>
+      </c>
+      <c r="F13">
         <v>-1.1569</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="4" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="7">
-        <v>6.293181</v>
-      </c>
-      <c r="C13" s="5">
-        <v>-1.120320181</v>
-      </c>
-      <c r="D13" s="5">
-        <v>-1.119</v>
-      </c>
-      <c r="E13" s="5">
-        <v>-1.1198</v>
-      </c>
-      <c r="F13" s="5">
+      <c r="B14" s="4">
+        <v>6.29318069901987</v>
+      </c>
+      <c r="C14">
+        <v>-1.12032018073023</v>
+      </c>
+      <c r="D14" s="5">
+        <v>-1.1295</v>
+      </c>
+      <c r="E14" s="6">
+        <v>-1.0744</v>
+      </c>
+      <c r="F14">
         <v>-1.1226</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="4" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="7">
-        <v>6.226863</v>
-      </c>
-      <c r="C14" s="5">
-        <v>-1.082144172</v>
-      </c>
-      <c r="D14" s="5">
-        <v>-1.0686</v>
-      </c>
-      <c r="E14" s="5">
-        <v>-1.0744</v>
-      </c>
-      <c r="F14" s="5">
+      <c r="B15" s="4">
+        <v>6.22686319173841</v>
+      </c>
+      <c r="C15">
+        <v>-1.08214417160377</v>
+      </c>
+      <c r="D15" s="5">
+        <v>-1.0829</v>
+      </c>
+      <c r="E15" s="6">
+        <v>-1.0162</v>
+      </c>
+      <c r="F15">
         <v>-1.077</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="4" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="7">
-        <v>6.160546</v>
-      </c>
-      <c r="C15" s="5">
-        <v>-1.034574247</v>
-      </c>
-      <c r="D15" s="5">
-        <v>-1.0038</v>
-      </c>
-      <c r="E15" s="5">
-        <v>-1.0162</v>
-      </c>
-      <c r="F15" s="5">
+      <c r="B16" s="4">
+        <v>6.16054568445696</v>
+      </c>
+      <c r="C16">
+        <v>-1.03457424671424</v>
+      </c>
+      <c r="D16" s="5">
+        <v>-1.0224</v>
+      </c>
+      <c r="E16" s="6">
+        <v>-0.9436</v>
+      </c>
+      <c r="F16">
         <v>-1.0184</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="4" t="s">
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="7">
-        <v>6.094228</v>
-      </c>
-      <c r="C16" s="5">
-        <v>-0.976615551</v>
-      </c>
-      <c r="D16" s="5">
-        <v>-0.9223</v>
-      </c>
-      <c r="E16" s="5">
-        <v>-0.9436</v>
-      </c>
-      <c r="F16" s="5">
+      <c r="B17" s="4">
+        <v>6.0942281771755</v>
+      </c>
+      <c r="C17">
+        <v>-0.976615550953454</v>
+      </c>
+      <c r="D17" s="5">
+        <v>-0.9461</v>
+      </c>
+      <c r="E17" s="5">
+        <v>-0.9461</v>
+      </c>
+      <c r="F17">
         <v>-0.9449</v>
       </c>
     </row>
@@ -53456,7 +53476,7 @@
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
         <v>57</v>
@@ -53747,7 +53767,7 @@
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
update data for shifted geofile
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -25,7 +25,6 @@
     <definedName name="res" localSheetId="5">down!$C$2:$C$16</definedName>
     <definedName name="res" localSheetId="6">up!$C$2:$C$16</definedName>
     <definedName name="res_1" localSheetId="5">down!$D$2:$D$16</definedName>
-    <definedName name="res_1" localSheetId="4">shift!$E$2:$E$16</definedName>
     <definedName name="res_1" localSheetId="6">up!$E$2:$E$16</definedName>
     <definedName name="res_2" localSheetId="5">down!$E$2:$E$16</definedName>
     <definedName name="res_2" localSheetId="6">up!$D$2:$D$16</definedName>
@@ -33,6 +32,7 @@
     <definedName name="tmp_1" localSheetId="2">CCmd!$L$2:$L$16</definedName>
     <definedName name="ExternalData_1" localSheetId="4">shift!$F$2:$F$17</definedName>
     <definedName name="ExternalData_2" localSheetId="4">shift!$D$2:$D$17</definedName>
+    <definedName name="ExternalData_3" localSheetId="4">shift!$E$2:$E$17</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
@@ -86,63 +86,63 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="res1" type="6" background="1" refreshedVersion="2" saveData="1">
+  <connection id="1" name="res3" type="6" background="1" refreshedVersion="2" saveData="1">
     <textPr sourceFile="/Users/yerong/Documents/William/res.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="res3" type="6" background="1" refreshedVersion="2" saveData="1">
+  <connection id="2" name="res4" type="6" background="1" refreshedVersion="2" saveData="1">
     <textPr sourceFile="/Users/yerong/Documents/William/res.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="res4" type="6" background="1" refreshedVersion="2" saveData="1">
+  <connection id="3" name="res5" type="6" background="1" refreshedVersion="2" saveData="1">
     <textPr sourceFile="/Users/yerong/Documents/William/res.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="res5" type="6" background="1" refreshedVersion="2" saveData="1">
+  <connection id="4" name="res6" type="6" background="1" refreshedVersion="2" saveData="1">
     <textPr sourceFile="/Users/yerong/Documents/William/res.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="res6" type="6" background="1" refreshedVersion="2" saveData="1">
+  <connection id="5" name="res7" type="6" background="1" refreshedVersion="2" saveData="1">
     <textPr sourceFile="/Users/yerong/Documents/William/res.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="res7" type="6" background="1" refreshedVersion="2" saveData="1">
+  <connection id="6" name="res8" type="6" background="1" refreshedVersion="2" saveData="1">
     <textPr sourceFile="/Users/yerong/Documents/William/res.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="res8" type="6" background="1" refreshedVersion="2" saveData="1">
-    <textPr sourceFile="/Users/yerong/Documents/William/res.txt">
-      <textFields>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="8" name="rst" type="6" background="1" refreshedVersion="2" saveData="1">
+  <connection id="7" name="rst" type="6" background="1" refreshedVersion="2" saveData="1">
     <textPr sourceFile="F:\William\rst.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="rst1" type="6" background="1" refreshedVersion="2" saveData="1">
+  <connection id="8" name="rst1" type="6" background="1" refreshedVersion="2" saveData="1">
+    <textPr sourceFile="F:\William\rst.txt">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="9" name="rst2" type="6" background="1" refreshedVersion="2" saveData="1">
     <textPr sourceFile="F:\William\rst.txt">
       <textFields>
         <textField/>
@@ -374,11 +374,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="0.000000"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="0.000000"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -405,13 +405,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -419,14 +412,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -436,7 +436,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -449,8 +449,16 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -464,17 +472,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -489,24 +504,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -525,16 +525,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -549,7 +549,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -564,7 +564,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -576,25 +582,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -612,19 +600,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -642,13 +642,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -660,91 +744,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -761,7 +761,81 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -781,225 +855,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1014,7 +1014,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1097,6 +1097,76 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_6" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
+    <queryTableFields count="1">
+      <queryTableField id="1" dataBound="0"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
+    <queryTableFields count="1">
+      <queryTableField id="1" dataBound="0"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
+    <queryTableFields count="1">
+      <queryTableField id="1" dataBound="0"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
+    <queryTableFields count="1">
+      <queryTableField id="1" dataBound="0"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
+    <queryTableFields count="1">
+      <queryTableField id="1" dataBound="0"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_5" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
+    <queryTableFields count="1">
+      <queryTableField id="1" dataBound="0"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_4" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
+    <queryTableFields count="1">
+      <queryTableField id="1" dataBound="0"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp_1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
@@ -1106,78 +1176,8 @@
 </queryTable>
 </file>
 
-<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
-    <queryTableFields count="1">
-      <queryTableField id="1" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
-    <queryTableFields count="1">
-      <queryTableField id="1" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
-    <queryTableFields count="1">
-      <queryTableField id="1" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
-    <queryTableFields count="1">
-      <queryTableField id="1" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_4" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
-    <queryTableFields count="1">
-      <queryTableField id="1" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_5" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
-    <queryTableFields count="1">
-      <queryTableField id="1" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_6" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
-    <queryTableFields count="1">
-      <queryTableField id="1" dataBound="0"/>
-    </queryTableFields>
-  </queryTableRefresh>
-</queryTable>
-</file>
-
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_3" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -1187,8 +1187,8 @@
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
     </queryTableFields>
@@ -1197,7 +1197,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -1207,7 +1207,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -1217,7 +1217,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -53107,13 +53107,12 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F17"/>
+      <selection activeCell="D2" sqref="D2:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="5"/>
   <cols>
-    <col min="4" max="4" width="8.375" customWidth="1"/>
-    <col min="6" max="6" width="8.375" customWidth="1"/>
+    <col min="4" max="6" width="8.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -53145,13 +53144,13 @@
         <v>-1.16397647235087</v>
       </c>
       <c r="D2" s="5">
-        <v>-1.1486</v>
+        <v>-1.1462</v>
       </c>
       <c r="E2" s="6">
         <v>-1.1308</v>
       </c>
       <c r="F2" s="5">
-        <v>-1.1301</v>
+        <v>-1.1269</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -53165,13 +53164,13 @@
         <v>-1.17477787803301</v>
       </c>
       <c r="D3" s="5">
-        <v>-1.1661</v>
+        <v>-1.1638</v>
       </c>
       <c r="E3" s="6">
         <v>-1.1528</v>
       </c>
       <c r="F3" s="5">
-        <v>-1.1529</v>
+        <v>-1.1499</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -53185,13 +53184,13 @@
         <v>-1.186285248709</v>
       </c>
       <c r="D4" s="5">
-        <v>-1.1811</v>
+        <v>-1.1789</v>
       </c>
       <c r="E4" s="6">
-        <v>-1.1703</v>
+        <v>-1.1704</v>
       </c>
       <c r="F4" s="5">
-        <v>-1.1709</v>
+        <v>-1.1681</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -53205,13 +53204,13 @@
         <v>-1.195119714459</v>
       </c>
       <c r="D5" s="5">
-        <v>-1.1932</v>
+        <v>-1.1911</v>
       </c>
       <c r="E5" s="6">
-        <v>-1.1851</v>
+        <v>-1.1852</v>
       </c>
       <c r="F5" s="5">
-        <v>-1.1862</v>
+        <v>-1.1835</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -53225,13 +53224,13 @@
         <v>-1.20178949653999</v>
       </c>
       <c r="D6" s="5">
-        <v>-1.2019</v>
+        <v>-1.2</v>
       </c>
       <c r="E6" s="6">
         <v>-1.1967</v>
       </c>
       <c r="F6" s="5">
-        <v>-1.1982</v>
+        <v>-1.1957</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -53245,13 +53244,13 @@
         <v>-1.20503708359101</v>
       </c>
       <c r="D7" s="5">
-        <v>-1.2068</v>
+        <v>-1.205</v>
       </c>
       <c r="E7" s="6">
         <v>-1.2044</v>
       </c>
       <c r="F7" s="5">
-        <v>-1.2063</v>
+        <v>-1.2041</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -53265,13 +53264,13 @@
         <v>-1.20522788652559</v>
       </c>
       <c r="D8" s="5">
-        <v>-1.2074</v>
+        <v>-1.2057</v>
       </c>
       <c r="E8" s="5">
         <v>-1.2058</v>
       </c>
       <c r="F8" s="5">
-        <v>-1.2079</v>
+        <v>-1.2057</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -53285,13 +53284,13 @@
         <v>-1.20415879448197</v>
       </c>
       <c r="D9" s="5">
-        <v>-1.2073</v>
+        <v>-1.2057</v>
       </c>
       <c r="E9" s="6">
         <v>-1.2076</v>
       </c>
       <c r="F9" s="5">
-        <v>-1.21</v>
+        <v>-1.208</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -53305,13 +53304,13 @@
         <v>-1.19905021115693</v>
       </c>
       <c r="D10" s="5">
-        <v>-1.2028</v>
+        <v>-1.2014</v>
       </c>
       <c r="E10" s="6">
         <v>-1.2055</v>
       </c>
       <c r="F10" s="5">
-        <v>-1.2083</v>
+        <v>-1.2065</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -53325,13 +53324,13 @@
         <v>-1.18886879867486</v>
       </c>
       <c r="D11" s="5">
-        <v>-1.1927</v>
+        <v>-1.1915</v>
       </c>
       <c r="E11" s="6">
-        <v>-1.1974</v>
+        <v>-1.1973</v>
       </c>
       <c r="F11" s="5">
-        <v>-1.2005</v>
+        <v>-1.199</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -53345,13 +53344,13 @@
         <v>-1.17288753288264</v>
       </c>
       <c r="D12" s="5">
-        <v>-1.1763</v>
+        <v>-1.1753</v>
       </c>
       <c r="E12" s="6">
-        <v>-1.1822</v>
+        <v>-1.1821</v>
       </c>
       <c r="F12" s="5">
-        <v>-1.1855</v>
+        <v>-1.1843</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -53365,13 +53364,13 @@
         <v>-1.15031135712294</v>
       </c>
       <c r="D13" s="5">
-        <v>-1.1529</v>
+        <v>-1.152</v>
       </c>
       <c r="E13" s="6">
         <v>-1.1588</v>
       </c>
       <c r="F13" s="5">
-        <v>-1.1622</v>
+        <v>-1.1613</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -53385,13 +53384,13 @@
         <v>-1.12032018073023</v>
       </c>
       <c r="D14" s="5">
-        <v>-1.1214</v>
+        <v>-1.1207</v>
       </c>
       <c r="E14" s="6">
         <v>-1.1261</v>
       </c>
       <c r="F14" s="5">
-        <v>-1.1294</v>
+        <v>-1.1288</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -53405,13 +53404,13 @@
         <v>-1.08214417160377</v>
       </c>
       <c r="D15" s="5">
-        <v>-1.0811</v>
+        <v>-1.0806</v>
       </c>
       <c r="E15" s="6">
-        <v>-1.0827</v>
+        <v>-1.0826</v>
       </c>
       <c r="F15" s="5">
-        <v>-1.0855</v>
+        <v>-1.0852</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -53425,13 +53424,13 @@
         <v>-1.03457424671424</v>
       </c>
       <c r="D16" s="5">
-        <v>-1.0309</v>
+        <v>-1.0306</v>
       </c>
       <c r="E16" s="6">
         <v>-1.0269</v>
       </c>
       <c r="F16" s="5">
-        <v>-1.0291</v>
+        <v>-1.029</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -53445,13 +53444,13 @@
         <v>-0.976615550953454</v>
       </c>
       <c r="D17" s="5">
-        <v>-0.9698</v>
+        <v>-0.9696</v>
       </c>
       <c r="E17" s="5">
         <v>-0.957</v>
       </c>
       <c r="F17" s="5">
-        <v>-0.958</v>
+        <v>-0.9582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vasp file for z01 z02
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -20,7 +20,6 @@
     <definedName name="ExternalData_2" localSheetId="2">CCmd!$K$2:$K$16</definedName>
     <definedName name="ExternalData_3" localSheetId="2">CCmd!$J$2:$J$16</definedName>
     <definedName name="ExternalData_5" localSheetId="2">CCmd!$K$2:$K$16</definedName>
-    <definedName name="ExternalData_6" localSheetId="2">CCmd!$J$2:$J$16</definedName>
     <definedName name="res" localSheetId="5">down!$C$2:$C$16</definedName>
     <definedName name="res" localSheetId="6">up!$C$2:$C$16</definedName>
     <definedName name="res_1" localSheetId="5">down!$D$2:$D$16</definedName>
@@ -32,6 +31,7 @@
     <definedName name="ExternalData_1" localSheetId="4">shift!$F$2:$F$17</definedName>
     <definedName name="ExternalData_2" localSheetId="4">shift!$D$2:$D$17</definedName>
     <definedName name="ExternalData_3" localSheetId="4">shift!$E$2:$E$17</definedName>
+    <definedName name="ExternalData_1_1" localSheetId="2">CCmd!$J$2:$J$17</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
@@ -148,15 +148,15 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="tmp3" type="6" background="1" refreshedVersion="2" saveData="1">
-    <textPr sourceFile="/Users/yerong/Documents/William/tmp/tmp.txt">
+  <connection id="10" name="rst3" type="6" background="1" refreshedVersion="2" saveData="1">
+    <textPr sourceFile="F:\William\rst.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" name="tmp4" type="6" background="1" refreshedVersion="2" saveData="1">
-    <textPr sourceFile="F:\William\tmp.txt" space="1" consecutive="1">
+  <connection id="11" name="tmp3" type="6" background="1" refreshedVersion="2" saveData="1">
+    <textPr sourceFile="/Users/yerong/Documents/William/tmp/tmp.txt">
       <textFields>
         <textField/>
       </textFields>
@@ -367,10 +367,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="0.000000"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -399,6 +399,28 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -406,19 +428,29 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -432,32 +464,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -472,7 +480,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -487,29 +495,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -518,7 +503,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -526,7 +511,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -534,14 +519,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -553,6 +553,30 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -574,19 +598,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -598,7 +664,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,13 +700,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -634,55 +724,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -694,49 +736,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -747,6 +747,41 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -774,17 +809,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -804,15 +833,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -827,171 +847,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1089,8 +1089,8 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp_1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1_1" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
     </queryTableFields>
@@ -1099,7 +1099,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -1119,7 +1119,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -1139,8 +1139,8 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_6" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tmp_1" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
     </queryTableFields>
@@ -1149,7 +1149,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_3" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -1169,7 +1169,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_3" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_2" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -1179,7 +1179,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -1199,7 +1199,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="res_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="1" nextId="2">
     <queryTableFields count="1">
       <queryTableField id="1" dataBound="0"/>
@@ -2670,7 +2670,7 @@
   <dimension ref="A1:M16384"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L17"/>
+      <selection activeCell="J2" sqref="J2:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -2683,7 +2683,7 @@
     <col min="7" max="7" width="10.3333333333333" customWidth="1"/>
     <col min="8" max="8" width="11.6666666666667" customWidth="1"/>
     <col min="9" max="9" width="12.875" customWidth="1"/>
-    <col min="10" max="10" width="12.1666666666667" customWidth="1"/>
+    <col min="10" max="10" width="14.375" customWidth="1"/>
     <col min="11" max="11" width="13.5" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
     <col min="13" max="13" width="16.1666666666667" customWidth="1"/>
@@ -2757,13 +2757,13 @@
         <v>-1.16397647235087</v>
       </c>
       <c r="J2" s="15">
-        <v>-1.1251</v>
+        <v>-1.1258</v>
       </c>
       <c r="K2" s="14">
         <v>-1.1812</v>
       </c>
       <c r="L2" s="15">
-        <v>-1.1215</v>
+        <v>-1.1205</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2795,13 +2795,13 @@
         <v>-1.17477787803301</v>
       </c>
       <c r="J3" s="15">
-        <v>-1.1475</v>
+        <v>-1.1482</v>
       </c>
       <c r="K3" s="14">
         <v>-1.2007</v>
       </c>
       <c r="L3" s="15">
-        <v>-1.1448</v>
+        <v>-1.1441</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2833,13 +2833,13 @@
         <v>-1.186285248709</v>
       </c>
       <c r="J4" s="15">
-        <v>-1.1654</v>
+        <v>-1.166</v>
       </c>
       <c r="K4" s="14">
         <v>-1.2173</v>
       </c>
       <c r="L4" s="15">
-        <v>-1.1632</v>
+        <v>-1.1626</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -2871,13 +2871,13 @@
         <v>-1.195119714459</v>
       </c>
       <c r="J5" s="15">
-        <v>-1.1805</v>
+        <v>-1.1811</v>
       </c>
       <c r="K5" s="14">
         <v>-1.2304</v>
       </c>
       <c r="L5" s="15">
-        <v>-1.1789</v>
+        <v>-1.1784</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -2909,13 +2909,13 @@
         <v>-1.20178949653999</v>
       </c>
       <c r="J6" s="15">
-        <v>-1.1924</v>
+        <v>-1.1929</v>
       </c>
       <c r="K6" s="14">
         <v>-1.2394</v>
       </c>
       <c r="L6" s="15">
-        <v>-1.1913</v>
+        <v>-1.191</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -2947,13 +2947,13 @@
         <v>-1.20503708359101</v>
       </c>
       <c r="J7" s="15">
-        <v>-1.2074</v>
+        <v>-1.2078</v>
       </c>
       <c r="K7" s="14">
         <v>-1.2435</v>
       </c>
       <c r="L7" s="15">
-        <v>-1.2078</v>
+        <v>-1.2077</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -2985,13 +2985,13 @@
         <v>-1.20522788652559</v>
       </c>
       <c r="J8" s="15">
-        <v>-1.2059</v>
+        <v>-1.2063</v>
       </c>
       <c r="K8" s="14">
         <v>0</v>
       </c>
       <c r="L8" s="15">
-        <v>-1.2063</v>
+        <v>-1.2062</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -3023,13 +3023,13 @@
         <v>-1.20415879448197</v>
       </c>
       <c r="J9" s="15">
-        <v>-1.204</v>
+        <v>-1.2044</v>
       </c>
       <c r="K9" s="14">
         <v>-1.2419</v>
       </c>
       <c r="L9" s="15">
-        <v>-1.2042</v>
+        <v>-1.2041</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -3061,13 +3061,13 @@
         <v>-1.19905021115693</v>
       </c>
       <c r="J10" s="15">
-        <v>-1.2024</v>
+        <v>-1.2027</v>
       </c>
       <c r="K10" s="14">
         <v>-1.2337</v>
       </c>
       <c r="L10" s="15">
-        <v>-1.2031</v>
+        <v>-1.2032</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -3099,13 +3099,13 @@
         <v>-1.18886879867486</v>
       </c>
       <c r="J11" s="15">
-        <v>-1.1946</v>
+        <v>-1.1949</v>
       </c>
       <c r="K11" s="14">
         <v>-1.2176</v>
       </c>
       <c r="L11" s="15">
-        <v>-1.1959</v>
+        <v>-1.1962</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -3137,13 +3137,13 @@
         <v>-1.17288753288264</v>
       </c>
       <c r="J12" s="15">
-        <v>-1.16</v>
+        <v>-1.1602</v>
       </c>
       <c r="K12" s="14">
         <v>-1.1925</v>
       </c>
       <c r="L12" s="15">
-        <v>-1.1623</v>
+        <v>-1.1628</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -3175,13 +3175,13 @@
         <v>-1.15031135712294</v>
       </c>
       <c r="J13" s="15">
-        <v>-1.157</v>
+        <v>-1.1572</v>
       </c>
       <c r="K13" s="14">
         <v>-1.1569</v>
       </c>
       <c r="L13" s="15">
-        <v>-1.1592</v>
+        <v>-1.1597</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -3213,13 +3213,13 @@
         <v>-1.12032018073023</v>
       </c>
       <c r="J14" s="15">
-        <v>-1.1249</v>
+        <v>-1.125</v>
       </c>
       <c r="K14" s="14">
         <v>-1.1092</v>
       </c>
       <c r="L14" s="15">
-        <v>-1.1272</v>
+        <v>-1.1278</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -3257,7 +3257,7 @@
         <v>-1.0475</v>
       </c>
       <c r="L15" s="15">
-        <v>-1.0843</v>
+        <v>-1.085</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -3295,7 +3295,7 @@
         <v>-0.9697</v>
       </c>
       <c r="L16" s="15">
-        <v>-1.0289</v>
+        <v>-1.0296</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:12">
@@ -3327,13 +3327,13 @@
         <v>-0.976615550953454</v>
       </c>
       <c r="J17" s="15">
-        <v>-0.9575</v>
+        <v>-0.9574</v>
       </c>
       <c r="K17" s="14">
         <v>-0.8734</v>
       </c>
       <c r="L17" s="15">
-        <v>-0.959</v>
+        <v>-0.9596</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="4:4">

</xml_diff>